<commit_message>
Updated DTP, Edited Playlist2, Exit to MainMenu
Update Version of DTP, with DTP done for graphicshandler. Edited
playlist 2 to play video. YSTV videos doesnt seems to load. Exit to
MainMenu via ESC key.
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="114">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -601,21 +601,12 @@
     <t>The Slideshow will be paused which means the Slide will stop displaying subsequent content until the next "Play" Button is pressed</t>
   </si>
   <si>
-    <t>Click on the Timer icon</t>
-  </si>
-  <si>
     <t>Set the duration for the Timer and click on the "Start" button in the timer display</t>
   </si>
   <si>
     <t>A digital timer is being displayed on top of the main menu window</t>
   </si>
   <si>
-    <t>The digital timer starts counting down based on the duration set. After the duration has passed, a beep sound is produced.</t>
-  </si>
-  <si>
-    <t>Import Shopping List</t>
-  </si>
-  <si>
     <t>Click on the "Recpies" Button and select the platform to retrieve recipes.</t>
   </si>
   <si>
@@ -638,6 +629,114 @@
   </si>
   <si>
     <t>Ingredients based on the selected CheckBoxes are displayed in the "Your Shopping List.pdf"</t>
+  </si>
+  <si>
+    <t>Timer returns to first selected duration</t>
+  </si>
+  <si>
+    <t>The digital timer starts counting down based on the duration set. Start button changes to pause.</t>
+  </si>
+  <si>
+    <t>Step 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The digital timer stops counting and remains at the same duration </t>
+  </si>
+  <si>
+    <t>Step 11</t>
+  </si>
+  <si>
+    <t>The digital timer resumes from the place it was paused</t>
+  </si>
+  <si>
+    <t>Step 12</t>
+  </si>
+  <si>
+    <t>Click the Create timer button</t>
+  </si>
+  <si>
+    <t>A second timer is created</t>
+  </si>
+  <si>
+    <t>Step 13</t>
+  </si>
+  <si>
+    <t>Repeat steps 7 - 11 for the second timer</t>
+  </si>
+  <si>
+    <t>Same results as 7-11</t>
+  </si>
+  <si>
+    <t>Step 14</t>
+  </si>
+  <si>
+    <t>Timers continue to count from same position before changing slide on the new slide</t>
+  </si>
+  <si>
+    <t>Step 15</t>
+  </si>
+  <si>
+    <t>Step 16</t>
+  </si>
+  <si>
+    <t>Click on the Create Timer Button</t>
+  </si>
+  <si>
+    <t>The digital timer starts counting down based on the duration set. Start button changes to pause After the duration has passed, a beep sound is produced.</t>
+  </si>
+  <si>
+    <t>Click the "Reset" Button</t>
+  </si>
+  <si>
+    <t>Click the "Start" Button</t>
+  </si>
+  <si>
+    <t>Click the "Pause" Button</t>
+  </si>
+  <si>
+    <t>Click the "Next Slide" Button</t>
+  </si>
+  <si>
+    <t>Click the "Previous Slide" Button</t>
+  </si>
+  <si>
+    <t>Timers reset to the timer that was originally selected</t>
+  </si>
+  <si>
+    <t>Create Shopping List</t>
+  </si>
+  <si>
+    <t>Store Notes</t>
+  </si>
+  <si>
+    <t>Move the mouse cursor to the left side of the screen</t>
+  </si>
+  <si>
+    <t>A notes panel will slide out from the left side of the screen</t>
+  </si>
+  <si>
+    <t>Insert some texts into the TextArea</t>
+  </si>
+  <si>
+    <t>Re-slide the notes panel. The notes panel should display what you have keyed in earlier on.</t>
+  </si>
+  <si>
+    <t>Navigate to the "Code" folder. Open up the eCook folder and search for "0_notes".txt file. Double click on the .txt file.</t>
+  </si>
+  <si>
+    <t>The .txt file should display what you have keyed into the notes panel.</t>
+  </si>
+  <si>
+    <t>Return to the Slideshow and Click on the "Next Slide" Button</t>
+  </si>
+  <si>
+    <t>A fullscreen slide window displaying shapes appears</t>
+  </si>
+  <si>
+    <t>Repeat steps 6-8. However, this time, search for "1_notes".txt file.</t>
+  </si>
+  <si>
+    <t>The .txt file should display what you have keyed into the notes panel in slide "1".</t>
   </si>
 </sst>
 </file>
@@ -719,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -746,9 +845,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -767,23 +863,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -794,14 +881,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:AA136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,97 +1204,98 @@
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="27"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
@@ -1200,102 +1307,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="15"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="E18" s="16"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
@@ -1307,65 +1415,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1377,7 +1485,7 @@
       <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1389,21 +1497,21 @@
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="18"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="4" t="s">
         <v>1</v>
       </c>
@@ -1415,65 +1523,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="16"/>
-    </row>
-    <row r="33" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="16"/>
-    </row>
-    <row r="35" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -1485,7 +1593,7 @@
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="16"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -1497,7 +1605,7 @@
       <c r="C37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="16"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
@@ -1509,20 +1617,20 @@
       <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="16"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="E39" s="16"/>
+      <c r="A39" s="15"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="16"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="4" t="s">
         <v>1</v>
       </c>
@@ -1530,69 +1638,67 @@
         <v>0</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E41" s="15"/>
+    </row>
+    <row r="42" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="16"/>
-    </row>
-    <row r="43" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="16"/>
-    </row>
-    <row r="44" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="16"/>
-    </row>
-    <row r="45" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="16"/>
-    </row>
-    <row r="46" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E45" s="15"/>
+    </row>
+    <row r="46" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="16"/>
+      <c r="E46" s="15"/>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
@@ -1604,7 +1710,7 @@
       <c r="C47" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="16"/>
+      <c r="E47" s="15"/>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -1616,7 +1722,7 @@
       <c r="C48" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="16"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
@@ -1628,7 +1734,7 @@
       <c r="C49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E49" s="16"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
@@ -1640,20 +1746,20 @@
       <c r="C50" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="16"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="E51" s="16"/>
+      <c r="A51" s="15"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="16"/>
+      <c r="E52" s="15"/>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="4" t="s">
         <v>1</v>
       </c>
@@ -1665,65 +1771,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="55" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="16"/>
-    </row>
-    <row r="56" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E55" s="15"/>
+    </row>
+    <row r="56" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="16"/>
-    </row>
-    <row r="57" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E56" s="15"/>
+    </row>
+    <row r="57" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="16"/>
-    </row>
-    <row r="58" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E57" s="15"/>
+    </row>
+    <row r="58" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="16"/>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -1735,7 +1841,7 @@
       <c r="C59" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E59" s="16"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
@@ -1747,7 +1853,7 @@
       <c r="C60" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="16"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
@@ -1759,19 +1865,19 @@
       <c r="C61" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="16"/>
+      <c r="E61" s="15"/>
     </row>
     <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E62" s="21"/>
-    </row>
-    <row r="63" spans="1:5" s="12" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
+      <c r="E62" s="15"/>
+    </row>
+    <row r="63" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E63" s="26"/>
+      <c r="E63" s="15"/>
     </row>
     <row r="64" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="4" t="s">
         <v>1</v>
       </c>
@@ -1779,71 +1885,69 @@
         <v>0</v>
       </c>
       <c r="D64" s="7"/>
-      <c r="E64" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E65" s="15"/>
+    </row>
+    <row r="66" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="16"/>
-    </row>
-    <row r="67" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E66" s="15"/>
+    </row>
+    <row r="67" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="18" t="s">
+      <c r="C67" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E67" s="16"/>
-    </row>
-    <row r="68" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="16"/>
-    </row>
-    <row r="69" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E68" s="15"/>
+    </row>
+    <row r="69" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="16"/>
-    </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E69" s="15"/>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -1853,9 +1957,9 @@
       <c r="C70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="16"/>
-    </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E70" s="15"/>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -1865,9 +1969,9 @@
       <c r="C71" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="16"/>
-    </row>
-    <row r="72" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="E71" s="15"/>
+    </row>
+    <row r="72" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -1877,379 +1981,1075 @@
       <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E72" s="16"/>
-    </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E73" s="16"/>
-    </row>
-    <row r="74" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A74" s="13" t="s">
+      <c r="E72" s="15"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="15"/>
+    </row>
+    <row r="74" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A74" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E74" s="22"/>
-    </row>
-    <row r="75" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="E74" s="15"/>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="18" t="s">
+      <c r="B76" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C76" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="16"/>
-    </row>
-    <row r="76" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+      <c r="E76" s="15"/>
+    </row>
+    <row r="77" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B77" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C77" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E76" s="16"/>
-    </row>
-    <row r="77" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+      <c r="E77" s="15"/>
+    </row>
+    <row r="78" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B78" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C78" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E77" s="16"/>
-    </row>
-    <row r="78" spans="1:5" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="E78" s="15"/>
+    </row>
+    <row r="79" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B79" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C79" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E78" s="16"/>
-    </row>
-    <row r="79" spans="1:5" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+      <c r="E79" s="15"/>
+    </row>
+    <row r="80" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B80" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C80" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E79" s="16"/>
-    </row>
-    <row r="80" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+      <c r="E80" s="15"/>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E80" s="16"/>
-    </row>
-    <row r="81" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="E81" s="15"/>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E81" s="16"/>
-    </row>
-    <row r="82" spans="1:5" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
+      <c r="E82" s="15"/>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E82" s="16"/>
-    </row>
-    <row r="83" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E83" s="16"/>
-    </row>
-    <row r="84" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A84" s="13" t="s">
+      <c r="E83" s="15"/>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="15"/>
+    </row>
+    <row r="85" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A85" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E84" s="22"/>
-    </row>
-    <row r="85" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
+      <c r="E85" s="15"/>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
+      <c r="B86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="7"/>
+      <c r="E86" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B87" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C85" s="25" t="s">
+      <c r="C87" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="27"/>
-    </row>
-    <row r="86" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
+      <c r="E87" s="15"/>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B88" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C86" s="25" t="s">
+      <c r="C88" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E86" s="27"/>
-    </row>
-    <row r="87" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+      <c r="E88" s="15"/>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B89" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C89" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E87" s="27"/>
-    </row>
-    <row r="88" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+      <c r="E89" s="15"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B90" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C90" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E88" s="27"/>
-    </row>
-    <row r="89" spans="1:5" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+      <c r="E90" s="15"/>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B91" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C89" s="24" t="s">
+      <c r="C91" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E89" s="27"/>
-    </row>
-    <row r="90" spans="1:5" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+      <c r="E91" s="15"/>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B92" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C92" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E90" s="27"/>
-    </row>
-    <row r="91" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="E92" s="15"/>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B93" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C93" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E91" s="27"/>
-    </row>
-    <row r="92" spans="1:5" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+      <c r="E93" s="15"/>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B94" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C94" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E92" s="27"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="22"/>
-    </row>
-    <row r="94" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A94" s="13" t="s">
+      <c r="E94" s="15"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="15"/>
+    </row>
+    <row r="96" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A96" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E94" s="22"/>
-    </row>
-    <row r="95" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="E96" s="15"/>
+    </row>
+    <row r="97" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="15"/>
+      <c r="B97" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B98" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C95" s="25" t="s">
+      <c r="C98" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="27"/>
-    </row>
-    <row r="96" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+      <c r="D98" s="26"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="26"/>
+      <c r="L98" s="26"/>
+      <c r="M98" s="26"/>
+      <c r="N98" s="26"/>
+      <c r="O98" s="26"/>
+      <c r="P98" s="26"/>
+      <c r="Q98" s="26"/>
+      <c r="R98" s="26"/>
+      <c r="S98" s="26"/>
+      <c r="T98" s="26"/>
+      <c r="U98" s="26"/>
+      <c r="V98" s="26"/>
+      <c r="W98" s="26"/>
+      <c r="X98" s="26"/>
+      <c r="Y98" s="26"/>
+      <c r="Z98" s="26"/>
+      <c r="AA98" s="26"/>
+    </row>
+    <row r="99" spans="1:27" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B99" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C96" s="25" t="s">
+      <c r="C99" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E96" s="27"/>
-    </row>
-    <row r="97" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+      <c r="D99" s="26"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="26"/>
+      <c r="K99" s="26"/>
+      <c r="L99" s="26"/>
+      <c r="M99" s="26"/>
+      <c r="N99" s="26"/>
+      <c r="O99" s="26"/>
+      <c r="P99" s="26"/>
+      <c r="Q99" s="26"/>
+      <c r="R99" s="26"/>
+      <c r="S99" s="26"/>
+      <c r="T99" s="26"/>
+      <c r="U99" s="26"/>
+      <c r="V99" s="26"/>
+      <c r="W99" s="26"/>
+      <c r="X99" s="26"/>
+      <c r="Y99" s="26"/>
+      <c r="Z99" s="26"/>
+      <c r="AA99" s="26"/>
+    </row>
+    <row r="100" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="24" t="s">
+      <c r="B100" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C97" s="24" t="s">
+      <c r="C100" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E97" s="27"/>
-    </row>
-    <row r="98" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="D100" s="26"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="26"/>
+      <c r="O100" s="26"/>
+      <c r="P100" s="26"/>
+      <c r="Q100" s="26"/>
+      <c r="R100" s="26"/>
+      <c r="S100" s="26"/>
+      <c r="T100" s="26"/>
+      <c r="U100" s="26"/>
+      <c r="V100" s="26"/>
+      <c r="W100" s="26"/>
+      <c r="X100" s="26"/>
+      <c r="Y100" s="26"/>
+      <c r="Z100" s="26"/>
+      <c r="AA100" s="26"/>
+    </row>
+    <row r="101" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B101" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C101" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" s="26"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="26"/>
+      <c r="M101" s="26"/>
+      <c r="N101" s="26"/>
+      <c r="O101" s="26"/>
+      <c r="P101" s="26"/>
+      <c r="Q101" s="26"/>
+      <c r="R101" s="26"/>
+      <c r="S101" s="26"/>
+      <c r="T101" s="26"/>
+      <c r="U101" s="26"/>
+      <c r="V101" s="26"/>
+      <c r="W101" s="26"/>
+      <c r="X101" s="26"/>
+      <c r="Y101" s="26"/>
+      <c r="Z101" s="26"/>
+      <c r="AA101" s="26"/>
+    </row>
+    <row r="102" spans="1:27" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" s="26"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="26"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="26"/>
+      <c r="I102" s="26"/>
+      <c r="J102" s="26"/>
+      <c r="K102" s="26"/>
+      <c r="L102" s="26"/>
+      <c r="M102" s="26"/>
+      <c r="N102" s="26"/>
+      <c r="O102" s="26"/>
+      <c r="P102" s="26"/>
+      <c r="Q102" s="26"/>
+      <c r="R102" s="26"/>
+      <c r="S102" s="26"/>
+      <c r="T102" s="26"/>
+      <c r="U102" s="26"/>
+      <c r="V102" s="26"/>
+      <c r="W102" s="26"/>
+      <c r="X102" s="26"/>
+      <c r="Y102" s="26"/>
+      <c r="Z102" s="26"/>
+      <c r="AA102" s="26"/>
+    </row>
+    <row r="103" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103" s="24"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="24"/>
+      <c r="K103" s="24"/>
+      <c r="L103" s="24"/>
+      <c r="M103" s="24"/>
+      <c r="N103" s="24"/>
+      <c r="O103" s="24"/>
+      <c r="P103" s="24"/>
+      <c r="Q103" s="24"/>
+      <c r="R103" s="24"/>
+      <c r="S103" s="24"/>
+      <c r="T103" s="24"/>
+      <c r="U103" s="24"/>
+      <c r="V103" s="24"/>
+      <c r="W103" s="24"/>
+      <c r="X103" s="24"/>
+      <c r="Y103" s="24"/>
+      <c r="Z103" s="24"/>
+      <c r="AA103" s="24"/>
+    </row>
+    <row r="104" spans="1:27" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C104" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D104" s="24"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="24"/>
+      <c r="N104" s="24"/>
+      <c r="O104" s="24"/>
+      <c r="P104" s="24"/>
+      <c r="Q104" s="24"/>
+      <c r="R104" s="24"/>
+      <c r="S104" s="24"/>
+      <c r="T104" s="24"/>
+      <c r="U104" s="24"/>
+      <c r="V104" s="24"/>
+      <c r="W104" s="24"/>
+      <c r="X104" s="24"/>
+      <c r="Y104" s="24"/>
+      <c r="Z104" s="24"/>
+      <c r="AA104" s="24"/>
+    </row>
+    <row r="105" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C105" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D105" s="24"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="24"/>
+      <c r="K105" s="24"/>
+      <c r="L105" s="24"/>
+      <c r="M105" s="24"/>
+      <c r="N105" s="24"/>
+      <c r="O105" s="24"/>
+      <c r="P105" s="24"/>
+      <c r="Q105" s="24"/>
+      <c r="R105" s="24"/>
+      <c r="S105" s="24"/>
+      <c r="T105" s="24"/>
+      <c r="U105" s="24"/>
+      <c r="V105" s="24"/>
+      <c r="W105" s="24"/>
+      <c r="X105" s="24"/>
+      <c r="Y105" s="24"/>
+      <c r="Z105" s="24"/>
+      <c r="AA105" s="24"/>
+    </row>
+    <row r="106" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C106" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D106" s="24"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+      <c r="I106" s="24"/>
+      <c r="J106" s="24"/>
+      <c r="K106" s="24"/>
+      <c r="L106" s="24"/>
+      <c r="M106" s="24"/>
+      <c r="N106" s="24"/>
+      <c r="O106" s="24"/>
+      <c r="P106" s="24"/>
+      <c r="Q106" s="24"/>
+      <c r="R106" s="24"/>
+      <c r="S106" s="24"/>
+      <c r="T106" s="24"/>
+      <c r="U106" s="24"/>
+      <c r="V106" s="24"/>
+      <c r="W106" s="24"/>
+      <c r="X106" s="24"/>
+      <c r="Y106" s="24"/>
+      <c r="Z106" s="24"/>
+      <c r="AA106" s="24"/>
+    </row>
+    <row r="107" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C107" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D107" s="24"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
+      <c r="I107" s="24"/>
+      <c r="J107" s="24"/>
+      <c r="K107" s="24"/>
+      <c r="L107" s="24"/>
+      <c r="M107" s="24"/>
+      <c r="N107" s="24"/>
+      <c r="O107" s="24"/>
+      <c r="P107" s="24"/>
+      <c r="Q107" s="24"/>
+      <c r="R107" s="24"/>
+      <c r="S107" s="24"/>
+      <c r="T107" s="24"/>
+      <c r="U107" s="24"/>
+      <c r="V107" s="24"/>
+      <c r="W107" s="24"/>
+      <c r="X107" s="24"/>
+      <c r="Y107" s="24"/>
+      <c r="Z107" s="24"/>
+      <c r="AA107" s="24"/>
+    </row>
+    <row r="108" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D108" s="24"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
+      <c r="I108" s="24"/>
+      <c r="J108" s="24"/>
+      <c r="K108" s="24"/>
+      <c r="L108" s="24"/>
+      <c r="M108" s="24"/>
+      <c r="N108" s="24"/>
+      <c r="O108" s="24"/>
+      <c r="P108" s="24"/>
+      <c r="Q108" s="24"/>
+      <c r="R108" s="24"/>
+      <c r="S108" s="24"/>
+      <c r="T108" s="24"/>
+      <c r="U108" s="24"/>
+      <c r="V108" s="24"/>
+      <c r="W108" s="24"/>
+      <c r="X108" s="24"/>
+      <c r="Y108" s="24"/>
+      <c r="Z108" s="24"/>
+      <c r="AA108" s="24"/>
+    </row>
+    <row r="109" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D109" s="24"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+      <c r="I109" s="24"/>
+      <c r="J109" s="24"/>
+      <c r="K109" s="24"/>
+      <c r="L109" s="24"/>
+      <c r="M109" s="24"/>
+      <c r="N109" s="24"/>
+      <c r="O109" s="24"/>
+      <c r="P109" s="24"/>
+      <c r="Q109" s="24"/>
+      <c r="R109" s="24"/>
+      <c r="S109" s="24"/>
+      <c r="T109" s="24"/>
+      <c r="U109" s="24"/>
+      <c r="V109" s="24"/>
+      <c r="W109" s="24"/>
+      <c r="X109" s="24"/>
+      <c r="Y109" s="24"/>
+      <c r="Z109" s="24"/>
+      <c r="AA109" s="24"/>
+    </row>
+    <row r="110" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D110" s="24"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
+      <c r="I110" s="24"/>
+      <c r="J110" s="24"/>
+      <c r="K110" s="24"/>
+      <c r="L110" s="24"/>
+      <c r="M110" s="24"/>
+      <c r="N110" s="24"/>
+      <c r="O110" s="24"/>
+      <c r="P110" s="24"/>
+      <c r="Q110" s="24"/>
+      <c r="R110" s="24"/>
+      <c r="S110" s="24"/>
+      <c r="T110" s="24"/>
+      <c r="U110" s="24"/>
+      <c r="V110" s="24"/>
+      <c r="W110" s="24"/>
+      <c r="X110" s="24"/>
+      <c r="Y110" s="24"/>
+      <c r="Z110" s="24"/>
+      <c r="AA110" s="24"/>
+    </row>
+    <row r="111" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C111" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D111" s="24"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
+      <c r="I111" s="24"/>
+      <c r="J111" s="24"/>
+      <c r="K111" s="24"/>
+      <c r="L111" s="24"/>
+      <c r="M111" s="24"/>
+      <c r="N111" s="24"/>
+      <c r="O111" s="24"/>
+      <c r="P111" s="24"/>
+      <c r="Q111" s="24"/>
+      <c r="R111" s="24"/>
+      <c r="S111" s="24"/>
+      <c r="T111" s="24"/>
+      <c r="U111" s="24"/>
+      <c r="V111" s="24"/>
+      <c r="W111" s="24"/>
+      <c r="X111" s="24"/>
+      <c r="Y111" s="24"/>
+      <c r="Z111" s="24"/>
+      <c r="AA111" s="24"/>
+    </row>
+    <row r="112" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C112" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D112" s="24"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="30"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
+      <c r="I112" s="24"/>
+      <c r="J112" s="24"/>
+      <c r="K112" s="24"/>
+      <c r="L112" s="24"/>
+      <c r="M112" s="24"/>
+      <c r="N112" s="24"/>
+      <c r="O112" s="24"/>
+      <c r="P112" s="24"/>
+      <c r="Q112" s="24"/>
+      <c r="R112" s="24"/>
+      <c r="S112" s="24"/>
+      <c r="T112" s="24"/>
+      <c r="U112" s="24"/>
+      <c r="V112" s="24"/>
+      <c r="W112" s="24"/>
+      <c r="X112" s="24"/>
+      <c r="Y112" s="24"/>
+      <c r="Z112" s="24"/>
+      <c r="AA112" s="24"/>
+    </row>
+    <row r="113" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C113" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D113" s="24"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+      <c r="I113" s="24"/>
+      <c r="J113" s="24"/>
+      <c r="K113" s="24"/>
+      <c r="L113" s="24"/>
+      <c r="M113" s="24"/>
+      <c r="N113" s="24"/>
+      <c r="O113" s="24"/>
+      <c r="P113" s="24"/>
+      <c r="Q113" s="24"/>
+      <c r="R113" s="24"/>
+      <c r="S113" s="24"/>
+      <c r="T113" s="24"/>
+      <c r="U113" s="24"/>
+      <c r="V113" s="24"/>
+      <c r="W113" s="24"/>
+      <c r="X113" s="24"/>
+      <c r="Y113" s="24"/>
+      <c r="Z113" s="24"/>
+      <c r="AA113" s="24"/>
+    </row>
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E114" s="15"/>
+    </row>
+    <row r="115" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A115" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E115" s="15"/>
+    </row>
+    <row r="116" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="15"/>
+      <c r="B116" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="7"/>
+      <c r="E116" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117" s="22"/>
+    </row>
+    <row r="118" spans="1:27" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E118" s="22"/>
+    </row>
+    <row r="119" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E119" s="22"/>
+    </row>
+    <row r="120" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E98" s="28"/>
-    </row>
-    <row r="99" spans="1:5" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+      <c r="C120" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E120" s="22"/>
+    </row>
+    <row r="121" spans="1:27" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A121" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E99" s="28"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="22"/>
-    </row>
-    <row r="101" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A101" s="13" t="s">
+      <c r="B121" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E101" s="22"/>
-    </row>
-    <row r="102" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+      <c r="C121" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E121" s="22"/>
+    </row>
+    <row r="122" spans="1:27" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E122" s="22"/>
+    </row>
+    <row r="123" spans="1:27" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E123" s="22"/>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E124" s="15"/>
+    </row>
+    <row r="125" spans="1:27" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A125" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E125" s="15"/>
+    </row>
+    <row r="126" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="15"/>
+      <c r="B126" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="7"/>
+      <c r="E126" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:27" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="24" t="s">
+      <c r="B127" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C102" s="25" t="s">
+      <c r="C127" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E102" s="27"/>
-    </row>
-    <row r="103" spans="1:5" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
+      <c r="E127" s="15"/>
+    </row>
+    <row r="128" spans="1:27" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B128" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C103" s="25" t="s">
+      <c r="C128" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E103" s="27"/>
-    </row>
-    <row r="104" spans="1:5" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+      <c r="E128" s="15"/>
+    </row>
+    <row r="129" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="24" t="s">
+      <c r="B129" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C104" s="24" t="s">
+      <c r="C129" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E104" s="27"/>
-    </row>
-    <row r="105" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
+      <c r="E129" s="15"/>
+    </row>
+    <row r="130" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C105" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E105" s="28"/>
-    </row>
-    <row r="106" spans="1:5" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+      <c r="B130" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E130" s="15"/>
+    </row>
+    <row r="131" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E106" s="28"/>
-    </row>
-    <row r="107" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="B131" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E131" s="15"/>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B107" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E107" s="27"/>
-    </row>
-    <row r="108" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+      <c r="B132" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E132" s="15"/>
+    </row>
+    <row r="133" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C108" s="10" t="s">
+      <c r="B133" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E133" s="15"/>
+    </row>
+    <row r="134" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E134" s="15"/>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E135" s="15"/>
+    </row>
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E108" s="27"/>
+      <c r="B136" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E136" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2259,10 +3059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +3072,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -2280,17 +3080,25 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="13"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>41772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="28">
+        <v>41773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DTP Record to include Shopping List
And completed DTP record for latest work on Main Menu pages (shopping
list and ingredients page).
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20500" windowHeight="7640"/>
   </bookViews>
   <sheets>
     <sheet name="DTP" sheetId="10" r:id="rId1"/>
     <sheet name="Documentation" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="115">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -607,27 +610,9 @@
     <t>A digital timer is being displayed on top of the main menu window</t>
   </si>
   <si>
-    <t>Click on the "Recpies" Button and select the platform to retrieve recipes.</t>
-  </si>
-  <si>
-    <t>Appropriate recipes retrieved from the selected platform are displayed.</t>
-  </si>
-  <si>
-    <t>Select a few CheckBoxes and click on the "Home" image located at top left hand corner to return to main menu. Click on the "Shopping List" Button.</t>
-  </si>
-  <si>
     <t>Ingredients based on the selected CheckBoxes are displayed in the "Shopping List" menu.</t>
   </si>
   <si>
-    <t xml:space="preserve">Click on the "Save Recpies" Button </t>
-  </si>
-  <si>
-    <t>The current Shopping List should appear in the Resources folder with it's filename "Your Shopping List.pdf"</t>
-  </si>
-  <si>
-    <t>Navigate to the location of the "Resources" folder which is inside the "Code" folder. Select one of the Playlist inside the "Resource" folder. Open up "Your Shopping List.pdf".</t>
-  </si>
-  <si>
     <t>Ingredients based on the selected CheckBoxes are displayed in the "Your Shopping List.pdf"</t>
   </si>
   <si>
@@ -737,13 +722,34 @@
   </si>
   <si>
     <t>The .txt file should display what you have keyed into the notes panel in slide "1".</t>
+  </si>
+  <si>
+    <t>Click on the "Ingredient Picker" Button and select the first recipe in the list on the LHS of the screen</t>
+  </si>
+  <si>
+    <t>Two example recipes are listed, the first is selected by default. Recipe Info and Ingredients are displayed.</t>
+  </si>
+  <si>
+    <t>Select a few CheckBoxes next to ingredients and click on the "Home" image located at top left hand corner to return to main menu. Click on the "Generate Shopping List" Button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the "Save" Button </t>
+  </si>
+  <si>
+    <t>The current Shopping List should appear in the Root project folder with it's filename "Your Shopping List.pdf"</t>
+  </si>
+  <si>
+    <t>Navigate to the location of the Root project folder which is inside the "Code/eCook" folder. Open up "Your Shopping List.pdf".</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +797,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -815,10 +837,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -839,12 +863,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -876,13 +894,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -909,8 +921,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -969,7 +986,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1004,7 +1021,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1181,7 +1198,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1191,111 +1208,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="20">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="15">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="23"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" s="15" customFormat="1" ht="42">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="15">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="20">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
@@ -1307,103 +1328,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" s="15" customFormat="1" ht="42">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" s="15" customFormat="1" ht="28">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="13"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" s="15" customFormat="1" ht="28">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="15">
       <c r="A18" s="4"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="20">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A20" s="13"/>
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
@@ -1415,67 +1436,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" s="15" customFormat="1" ht="42">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="15">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1485,9 +1506,9 @@
       <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -1497,21 +1518,21 @@
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" customFormat="1">
+      <c r="A28" s="16"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="20">
       <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="B29" s="11"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A30" s="13"/>
       <c r="B30" s="4" t="s">
         <v>1</v>
       </c>
@@ -1523,67 +1544,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="1:5" s="15" customFormat="1" ht="42">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="15"/>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="15">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -1593,9 +1614,9 @@
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="15"/>
-    </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
@@ -1605,9 +1626,9 @@
       <c r="C37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="15"/>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="56">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1617,20 +1638,20 @@
       <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1">
+      <c r="A39" s="13"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="20">
       <c r="A40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="15"/>
-    </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A41" s="13"/>
       <c r="B41" s="4" t="s">
         <v>1</v>
       </c>
@@ -1638,69 +1659,69 @@
         <v>0</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A42" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E42" s="13"/>
+    </row>
+    <row r="43" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E43" s="13"/>
+    </row>
+    <row r="44" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E44" s="13"/>
+    </row>
+    <row r="45" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="15"/>
-    </row>
-    <row r="46" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" spans="1:5" s="15" customFormat="1" ht="42">
       <c r="A46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1710,9 +1731,9 @@
       <c r="C47" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E47" s="13"/>
+    </row>
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
@@ -1722,9 +1743,9 @@
       <c r="C48" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E48" s="13"/>
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A49" s="4" t="s">
         <v>9</v>
       </c>
@@ -1734,9 +1755,9 @@
       <c r="C49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E49" s="13"/>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -1746,20 +1767,20 @@
       <c r="C50" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="1:5" s="3" customFormat="1">
+      <c r="A51" s="13"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="20">
       <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A53" s="13"/>
       <c r="B53" s="4" t="s">
         <v>1</v>
       </c>
@@ -1771,67 +1792,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="15"/>
-    </row>
-    <row r="56" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E55" s="13"/>
+    </row>
+    <row r="56" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="15"/>
-    </row>
-    <row r="57" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="15"/>
-    </row>
-    <row r="58" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" spans="1:5" s="15" customFormat="1" ht="42">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="15"/>
-    </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="15">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -1841,9 +1862,9 @@
       <c r="C59" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E59" s="15"/>
-    </row>
-    <row r="60" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E59" s="13"/>
+    </row>
+    <row r="60" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -1853,9 +1874,9 @@
       <c r="C60" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="15"/>
-    </row>
-    <row r="61" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E60" s="13"/>
+    </row>
+    <row r="61" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A61" s="4" t="s">
         <v>9</v>
       </c>
@@ -1865,19 +1886,19 @@
       <c r="C61" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="15"/>
-    </row>
-    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" spans="1:5" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+      <c r="E61" s="13"/>
+    </row>
+    <row r="62" spans="1:5" customFormat="1">
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" spans="1:5" s="9" customFormat="1" ht="23">
+      <c r="A63" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+      <c r="E63" s="13"/>
+    </row>
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="A64" s="13"/>
       <c r="B64" s="4" t="s">
         <v>1</v>
       </c>
@@ -1885,69 +1906,69 @@
         <v>0</v>
       </c>
       <c r="D64" s="7"/>
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A65" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="15"/>
-    </row>
-    <row r="66" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="15"/>
-    </row>
-    <row r="67" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="15"/>
-    </row>
-    <row r="69" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" spans="1:6" s="15" customFormat="1" ht="42">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="15"/>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="15">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -1957,9 +1978,9 @@
       <c r="C70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E70" s="13"/>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="28">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -1969,9 +1990,9 @@
       <c r="C71" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="15"/>
-    </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" spans="1:6" s="3" customFormat="1" ht="56">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -1981,20 +2002,20 @@
       <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E72" s="15"/>
+      <c r="E72" s="13"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A74" s="12" t="s">
+    <row r="73" spans="1:6" s="3" customFormat="1">
+      <c r="E73" s="13"/>
+    </row>
+    <row r="74" spans="1:6" ht="23">
+      <c r="A74" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
+      <c r="E74" s="13"/>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="A75" s="13"/>
       <c r="B75" s="4" t="s">
         <v>1</v>
       </c>
@@ -2006,67 +2027,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A76" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="1:6" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E78" s="13"/>
+    </row>
+    <row r="79" spans="1:6" s="15" customFormat="1" ht="15">
       <c r="A79" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C79" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E79" s="15"/>
-    </row>
-    <row r="80" spans="1:6" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E79" s="13"/>
+    </row>
+    <row r="80" spans="1:6" s="15" customFormat="1" ht="42">
       <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E80" s="15"/>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E80" s="13"/>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="15">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -2076,9 +2097,9 @@
       <c r="C81" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E81" s="15"/>
-    </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E81" s="13"/>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" ht="28">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
@@ -2088,9 +2109,9 @@
       <c r="C82" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="15"/>
-    </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E82" s="13"/>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A83" s="4" t="s">
         <v>9</v>
       </c>
@@ -2100,19 +2121,19 @@
       <c r="C83" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E83" s="15"/>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A85" s="12" t="s">
+      <c r="E83" s="13"/>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1">
+      <c r="E84" s="13"/>
+    </row>
+    <row r="85" spans="1:6" ht="23">
+      <c r="A85" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E85" s="15"/>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
+      <c r="E85" s="13"/>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="A86" s="13"/>
       <c r="B86" s="4" t="s">
         <v>1</v>
       </c>
@@ -2124,7 +2145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
         <v>2</v>
       </c>
@@ -2134,9 +2155,9 @@
       <c r="C87" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="15"/>
-    </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E87" s="13"/>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -2146,9 +2167,9 @@
       <c r="C88" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="15"/>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E88" s="13"/>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1">
       <c r="A89" s="3" t="s">
         <v>4</v>
       </c>
@@ -2158,9 +2179,9 @@
       <c r="C89" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E89" s="15"/>
-    </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E89" s="13"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
@@ -2170,9 +2191,9 @@
       <c r="C90" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E90" s="15"/>
-    </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E90" s="13"/>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A91" s="3" t="s">
         <v>6</v>
       </c>
@@ -2182,9 +2203,9 @@
       <c r="C91" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E91" s="15"/>
-    </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E91" s="13"/>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1">
       <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
@@ -2194,9 +2215,9 @@
       <c r="C92" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E92" s="15"/>
-    </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="E92" s="13"/>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="28">
       <c r="A93" s="3" t="s">
         <v>7</v>
       </c>
@@ -2206,9 +2227,9 @@
       <c r="C93" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E93" s="15"/>
-    </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E93" s="13"/>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A94" s="3" t="s">
         <v>8</v>
       </c>
@@ -2218,20 +2239,20 @@
       <c r="C94" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E94" s="15"/>
+      <c r="E94" s="13"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E95" s="15"/>
-    </row>
-    <row r="96" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A96" s="12" t="s">
+    <row r="95" spans="1:6">
+      <c r="E95" s="13"/>
+    </row>
+    <row r="96" spans="1:6" ht="23">
+      <c r="A96" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E96" s="15"/>
-    </row>
-    <row r="97" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
+      <c r="E96" s="13"/>
+    </row>
+    <row r="97" spans="1:27" s="3" customFormat="1" ht="15">
+      <c r="A97" s="13"/>
       <c r="B97" s="4" t="s">
         <v>1</v>
       </c>
@@ -2243,577 +2264,577 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="23" t="s">
+    <row r="98" spans="1:27" s="18" customFormat="1" ht="15">
+      <c r="A98" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B98" s="25" t="s">
+      <c r="B98" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="26" t="s">
+      <c r="C98" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D98" s="26"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="26"/>
-      <c r="J98" s="26"/>
-      <c r="K98" s="26"/>
-      <c r="L98" s="26"/>
-      <c r="M98" s="26"/>
-      <c r="N98" s="26"/>
-      <c r="O98" s="26"/>
-      <c r="P98" s="26"/>
-      <c r="Q98" s="26"/>
-      <c r="R98" s="26"/>
-      <c r="S98" s="26"/>
-      <c r="T98" s="26"/>
-      <c r="U98" s="26"/>
-      <c r="V98" s="26"/>
-      <c r="W98" s="26"/>
-      <c r="X98" s="26"/>
-      <c r="Y98" s="26"/>
-      <c r="Z98" s="26"/>
-      <c r="AA98" s="26"/>
-    </row>
-    <row r="99" spans="1:27" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="23" t="s">
+      <c r="D98" s="22"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="22"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="22"/>
+      <c r="N98" s="22"/>
+      <c r="O98" s="22"/>
+      <c r="P98" s="22"/>
+      <c r="Q98" s="22"/>
+      <c r="R98" s="22"/>
+      <c r="S98" s="22"/>
+      <c r="T98" s="22"/>
+      <c r="U98" s="22"/>
+      <c r="V98" s="22"/>
+      <c r="W98" s="22"/>
+      <c r="X98" s="22"/>
+      <c r="Y98" s="22"/>
+      <c r="Z98" s="22"/>
+      <c r="AA98" s="22"/>
+    </row>
+    <row r="99" spans="1:27" s="18" customFormat="1" ht="15">
+      <c r="A99" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C99" s="26" t="s">
+      <c r="C99" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="26"/>
-      <c r="E99" s="15"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="26"/>
-      <c r="J99" s="26"/>
-      <c r="K99" s="26"/>
-      <c r="L99" s="26"/>
-      <c r="M99" s="26"/>
-      <c r="N99" s="26"/>
-      <c r="O99" s="26"/>
-      <c r="P99" s="26"/>
-      <c r="Q99" s="26"/>
-      <c r="R99" s="26"/>
-      <c r="S99" s="26"/>
-      <c r="T99" s="26"/>
-      <c r="U99" s="26"/>
-      <c r="V99" s="26"/>
-      <c r="W99" s="26"/>
-      <c r="X99" s="26"/>
-      <c r="Y99" s="26"/>
-      <c r="Z99" s="26"/>
-      <c r="AA99" s="26"/>
-    </row>
-    <row r="100" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="23" t="s">
+      <c r="D99" s="22"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="22"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="22"/>
+      <c r="N99" s="22"/>
+      <c r="O99" s="22"/>
+      <c r="P99" s="22"/>
+      <c r="Q99" s="22"/>
+      <c r="R99" s="22"/>
+      <c r="S99" s="22"/>
+      <c r="T99" s="22"/>
+      <c r="U99" s="22"/>
+      <c r="V99" s="22"/>
+      <c r="W99" s="22"/>
+      <c r="X99" s="22"/>
+      <c r="Y99" s="22"/>
+      <c r="Z99" s="22"/>
+      <c r="AA99" s="22"/>
+    </row>
+    <row r="100" spans="1:27" s="18" customFormat="1" ht="15">
+      <c r="A100" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="B100" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="C100" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D100" s="26"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="26"/>
-      <c r="G100" s="26"/>
-      <c r="H100" s="26"/>
-      <c r="I100" s="26"/>
-      <c r="J100" s="26"/>
-      <c r="K100" s="26"/>
-      <c r="L100" s="26"/>
-      <c r="M100" s="26"/>
-      <c r="N100" s="26"/>
-      <c r="O100" s="26"/>
-      <c r="P100" s="26"/>
-      <c r="Q100" s="26"/>
-      <c r="R100" s="26"/>
-      <c r="S100" s="26"/>
-      <c r="T100" s="26"/>
-      <c r="U100" s="26"/>
-      <c r="V100" s="26"/>
-      <c r="W100" s="26"/>
-      <c r="X100" s="26"/>
-      <c r="Y100" s="26"/>
-      <c r="Z100" s="26"/>
-      <c r="AA100" s="26"/>
-    </row>
-    <row r="101" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="23" t="s">
+      <c r="D100" s="22"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+      <c r="J100" s="22"/>
+      <c r="K100" s="22"/>
+      <c r="L100" s="22"/>
+      <c r="M100" s="22"/>
+      <c r="N100" s="22"/>
+      <c r="O100" s="22"/>
+      <c r="P100" s="22"/>
+      <c r="Q100" s="22"/>
+      <c r="R100" s="22"/>
+      <c r="S100" s="22"/>
+      <c r="T100" s="22"/>
+      <c r="U100" s="22"/>
+      <c r="V100" s="22"/>
+      <c r="W100" s="22"/>
+      <c r="X100" s="22"/>
+      <c r="Y100" s="22"/>
+      <c r="Z100" s="22"/>
+      <c r="AA100" s="22"/>
+    </row>
+    <row r="101" spans="1:27" s="18" customFormat="1" ht="15">
+      <c r="A101" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B101" s="25" t="s">
+      <c r="B101" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="25" t="s">
+      <c r="C101" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D101" s="26"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="26"/>
-      <c r="H101" s="26"/>
-      <c r="I101" s="26"/>
-      <c r="J101" s="26"/>
-      <c r="K101" s="26"/>
-      <c r="L101" s="26"/>
-      <c r="M101" s="26"/>
-      <c r="N101" s="26"/>
-      <c r="O101" s="26"/>
-      <c r="P101" s="26"/>
-      <c r="Q101" s="26"/>
-      <c r="R101" s="26"/>
-      <c r="S101" s="26"/>
-      <c r="T101" s="26"/>
-      <c r="U101" s="26"/>
-      <c r="V101" s="26"/>
-      <c r="W101" s="26"/>
-      <c r="X101" s="26"/>
-      <c r="Y101" s="26"/>
-      <c r="Z101" s="26"/>
-      <c r="AA101" s="26"/>
-    </row>
-    <row r="102" spans="1:27" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="23" t="s">
+      <c r="D101" s="22"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22"/>
+      <c r="I101" s="22"/>
+      <c r="J101" s="22"/>
+      <c r="K101" s="22"/>
+      <c r="L101" s="22"/>
+      <c r="M101" s="22"/>
+      <c r="N101" s="22"/>
+      <c r="O101" s="22"/>
+      <c r="P101" s="22"/>
+      <c r="Q101" s="22"/>
+      <c r="R101" s="22"/>
+      <c r="S101" s="22"/>
+      <c r="T101" s="22"/>
+      <c r="U101" s="22"/>
+      <c r="V101" s="22"/>
+      <c r="W101" s="22"/>
+      <c r="X101" s="22"/>
+      <c r="Y101" s="22"/>
+      <c r="Z101" s="22"/>
+      <c r="AA101" s="22"/>
+    </row>
+    <row r="102" spans="1:27" s="18" customFormat="1" ht="42">
+      <c r="A102" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="25" t="s">
+      <c r="B102" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C102" s="25" t="s">
+      <c r="C102" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D102" s="26"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="26"/>
-      <c r="G102" s="26"/>
-      <c r="H102" s="26"/>
-      <c r="I102" s="26"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="26"/>
-      <c r="L102" s="26"/>
-      <c r="M102" s="26"/>
-      <c r="N102" s="26"/>
-      <c r="O102" s="26"/>
-      <c r="P102" s="26"/>
-      <c r="Q102" s="26"/>
-      <c r="R102" s="26"/>
-      <c r="S102" s="26"/>
-      <c r="T102" s="26"/>
-      <c r="U102" s="26"/>
-      <c r="V102" s="26"/>
-      <c r="W102" s="26"/>
-      <c r="X102" s="26"/>
-      <c r="Y102" s="26"/>
-      <c r="Z102" s="26"/>
-      <c r="AA102" s="26"/>
-    </row>
-    <row r="103" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="23" t="s">
+      <c r="D102" s="22"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="22"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="22"/>
+      <c r="L102" s="22"/>
+      <c r="M102" s="22"/>
+      <c r="N102" s="22"/>
+      <c r="O102" s="22"/>
+      <c r="P102" s="22"/>
+      <c r="Q102" s="22"/>
+      <c r="R102" s="22"/>
+      <c r="S102" s="22"/>
+      <c r="T102" s="22"/>
+      <c r="U102" s="22"/>
+      <c r="V102" s="22"/>
+      <c r="W102" s="22"/>
+      <c r="X102" s="22"/>
+      <c r="Y102" s="22"/>
+      <c r="Z102" s="22"/>
+      <c r="AA102" s="22"/>
+    </row>
+    <row r="103" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A103" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C103" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103" s="20"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="20"/>
+      <c r="I103" s="20"/>
+      <c r="J103" s="20"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="20"/>
+      <c r="M103" s="20"/>
+      <c r="N103" s="20"/>
+      <c r="O103" s="20"/>
+      <c r="P103" s="20"/>
+      <c r="Q103" s="20"/>
+      <c r="R103" s="20"/>
+      <c r="S103" s="20"/>
+      <c r="T103" s="20"/>
+      <c r="U103" s="20"/>
+      <c r="V103" s="20"/>
+      <c r="W103" s="20"/>
+      <c r="X103" s="20"/>
+      <c r="Y103" s="20"/>
+      <c r="Z103" s="20"/>
+      <c r="AA103" s="20"/>
+    </row>
+    <row r="104" spans="1:27" s="8" customFormat="1" ht="42">
+      <c r="A104" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D104" s="20"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="20"/>
+      <c r="J104" s="20"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="20"/>
+      <c r="M104" s="20"/>
+      <c r="N104" s="20"/>
+      <c r="O104" s="20"/>
+      <c r="P104" s="20"/>
+      <c r="Q104" s="20"/>
+      <c r="R104" s="20"/>
+      <c r="S104" s="20"/>
+      <c r="T104" s="20"/>
+      <c r="U104" s="20"/>
+      <c r="V104" s="20"/>
+      <c r="W104" s="20"/>
+      <c r="X104" s="20"/>
+      <c r="Y104" s="20"/>
+      <c r="Z104" s="20"/>
+      <c r="AA104" s="20"/>
+    </row>
+    <row r="105" spans="1:27" s="8" customFormat="1" ht="15">
+      <c r="A105" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C105" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D105" s="20"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
+      <c r="J105" s="20"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="20"/>
+      <c r="M105" s="20"/>
+      <c r="N105" s="20"/>
+      <c r="O105" s="20"/>
+      <c r="P105" s="20"/>
+      <c r="Q105" s="20"/>
+      <c r="R105" s="20"/>
+      <c r="S105" s="20"/>
+      <c r="T105" s="20"/>
+      <c r="U105" s="20"/>
+      <c r="V105" s="20"/>
+      <c r="W105" s="20"/>
+      <c r="X105" s="20"/>
+      <c r="Y105" s="20"/>
+      <c r="Z105" s="20"/>
+      <c r="AA105" s="20"/>
+    </row>
+    <row r="106" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A106" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D106" s="20"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
+      <c r="I106" s="20"/>
+      <c r="J106" s="20"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="20"/>
+      <c r="M106" s="20"/>
+      <c r="N106" s="20"/>
+      <c r="O106" s="20"/>
+      <c r="P106" s="20"/>
+      <c r="Q106" s="20"/>
+      <c r="R106" s="20"/>
+      <c r="S106" s="20"/>
+      <c r="T106" s="20"/>
+      <c r="U106" s="20"/>
+      <c r="V106" s="20"/>
+      <c r="W106" s="20"/>
+      <c r="X106" s="20"/>
+      <c r="Y106" s="20"/>
+      <c r="Z106" s="20"/>
+      <c r="AA106" s="20"/>
+    </row>
+    <row r="107" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A107" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D107" s="20"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
+      <c r="I107" s="20"/>
+      <c r="J107" s="20"/>
+      <c r="K107" s="20"/>
+      <c r="L107" s="20"/>
+      <c r="M107" s="20"/>
+      <c r="N107" s="20"/>
+      <c r="O107" s="20"/>
+      <c r="P107" s="20"/>
+      <c r="Q107" s="20"/>
+      <c r="R107" s="20"/>
+      <c r="S107" s="20"/>
+      <c r="T107" s="20"/>
+      <c r="U107" s="20"/>
+      <c r="V107" s="20"/>
+      <c r="W107" s="20"/>
+      <c r="X107" s="20"/>
+      <c r="Y107" s="20"/>
+      <c r="Z107" s="20"/>
+      <c r="AA107" s="20"/>
+    </row>
+    <row r="108" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A108" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C108" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D108" s="20"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+      <c r="I108" s="20"/>
+      <c r="J108" s="20"/>
+      <c r="K108" s="20"/>
+      <c r="L108" s="20"/>
+      <c r="M108" s="20"/>
+      <c r="N108" s="20"/>
+      <c r="O108" s="20"/>
+      <c r="P108" s="20"/>
+      <c r="Q108" s="20"/>
+      <c r="R108" s="20"/>
+      <c r="S108" s="20"/>
+      <c r="T108" s="20"/>
+      <c r="U108" s="20"/>
+      <c r="V108" s="20"/>
+      <c r="W108" s="20"/>
+      <c r="X108" s="20"/>
+      <c r="Y108" s="20"/>
+      <c r="Z108" s="20"/>
+      <c r="AA108" s="20"/>
+    </row>
+    <row r="109" spans="1:27" s="8" customFormat="1" ht="15">
+      <c r="A109" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20"/>
+      <c r="I109" s="20"/>
+      <c r="J109" s="20"/>
+      <c r="K109" s="20"/>
+      <c r="L109" s="20"/>
+      <c r="M109" s="20"/>
+      <c r="N109" s="20"/>
+      <c r="O109" s="20"/>
+      <c r="P109" s="20"/>
+      <c r="Q109" s="20"/>
+      <c r="R109" s="20"/>
+      <c r="S109" s="20"/>
+      <c r="T109" s="20"/>
+      <c r="U109" s="20"/>
+      <c r="V109" s="20"/>
+      <c r="W109" s="20"/>
+      <c r="X109" s="20"/>
+      <c r="Y109" s="20"/>
+      <c r="Z109" s="20"/>
+      <c r="AA109" s="20"/>
+    </row>
+    <row r="110" spans="1:27" s="8" customFormat="1" ht="15">
+      <c r="A110" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D110" s="20"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="20"/>
+      <c r="I110" s="20"/>
+      <c r="J110" s="20"/>
+      <c r="K110" s="20"/>
+      <c r="L110" s="20"/>
+      <c r="M110" s="20"/>
+      <c r="N110" s="20"/>
+      <c r="O110" s="20"/>
+      <c r="P110" s="20"/>
+      <c r="Q110" s="20"/>
+      <c r="R110" s="20"/>
+      <c r="S110" s="20"/>
+      <c r="T110" s="20"/>
+      <c r="U110" s="20"/>
+      <c r="V110" s="20"/>
+      <c r="W110" s="20"/>
+      <c r="X110" s="20"/>
+      <c r="Y110" s="20"/>
+      <c r="Z110" s="20"/>
+      <c r="AA110" s="20"/>
+    </row>
+    <row r="111" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A111" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C111" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D111" s="20"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
+      <c r="J111" s="20"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="20"/>
+      <c r="M111" s="20"/>
+      <c r="N111" s="20"/>
+      <c r="O111" s="20"/>
+      <c r="P111" s="20"/>
+      <c r="Q111" s="20"/>
+      <c r="R111" s="20"/>
+      <c r="S111" s="20"/>
+      <c r="T111" s="20"/>
+      <c r="U111" s="20"/>
+      <c r="V111" s="20"/>
+      <c r="W111" s="20"/>
+      <c r="X111" s="20"/>
+      <c r="Y111" s="20"/>
+      <c r="Z111" s="20"/>
+      <c r="AA111" s="20"/>
+    </row>
+    <row r="112" spans="1:27" s="8" customFormat="1" ht="28">
+      <c r="A112" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C103" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D103" s="24"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
-      <c r="I103" s="24"/>
-      <c r="J103" s="24"/>
-      <c r="K103" s="24"/>
-      <c r="L103" s="24"/>
-      <c r="M103" s="24"/>
-      <c r="N103" s="24"/>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24"/>
-      <c r="Q103" s="24"/>
-      <c r="R103" s="24"/>
-      <c r="S103" s="24"/>
-      <c r="T103" s="24"/>
-      <c r="U103" s="24"/>
-      <c r="V103" s="24"/>
-      <c r="W103" s="24"/>
-      <c r="X103" s="24"/>
-      <c r="Y103" s="24"/>
-      <c r="Z103" s="24"/>
-      <c r="AA103" s="24"/>
-    </row>
-    <row r="104" spans="1:27" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A104" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C104" s="24" t="s">
+      <c r="C112" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D112" s="20"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="26"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="20"/>
+      <c r="I112" s="20"/>
+      <c r="J112" s="20"/>
+      <c r="K112" s="20"/>
+      <c r="L112" s="20"/>
+      <c r="M112" s="20"/>
+      <c r="N112" s="20"/>
+      <c r="O112" s="20"/>
+      <c r="P112" s="20"/>
+      <c r="Q112" s="20"/>
+      <c r="R112" s="20"/>
+      <c r="S112" s="20"/>
+      <c r="T112" s="20"/>
+      <c r="U112" s="20"/>
+      <c r="V112" s="20"/>
+      <c r="W112" s="20"/>
+      <c r="X112" s="20"/>
+      <c r="Y112" s="20"/>
+      <c r="Z112" s="20"/>
+      <c r="AA112" s="20"/>
+    </row>
+    <row r="113" spans="1:27" s="8" customFormat="1" ht="15">
+      <c r="A113" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C113" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D104" s="24"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
-      <c r="I104" s="24"/>
-      <c r="J104" s="24"/>
-      <c r="K104" s="24"/>
-      <c r="L104" s="24"/>
-      <c r="M104" s="24"/>
-      <c r="N104" s="24"/>
-      <c r="O104" s="24"/>
-      <c r="P104" s="24"/>
-      <c r="Q104" s="24"/>
-      <c r="R104" s="24"/>
-      <c r="S104" s="24"/>
-      <c r="T104" s="24"/>
-      <c r="U104" s="24"/>
-      <c r="V104" s="24"/>
-      <c r="W104" s="24"/>
-      <c r="X104" s="24"/>
-      <c r="Y104" s="24"/>
-      <c r="Z104" s="24"/>
-      <c r="AA104" s="24"/>
-    </row>
-    <row r="105" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B105" s="11" t="s">
+      <c r="D113" s="20"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+      <c r="I113" s="20"/>
+      <c r="J113" s="20"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="20"/>
+      <c r="M113" s="20"/>
+      <c r="N113" s="20"/>
+      <c r="O113" s="20"/>
+      <c r="P113" s="20"/>
+      <c r="Q113" s="20"/>
+      <c r="R113" s="20"/>
+      <c r="S113" s="20"/>
+      <c r="T113" s="20"/>
+      <c r="U113" s="20"/>
+      <c r="V113" s="20"/>
+      <c r="W113" s="20"/>
+      <c r="X113" s="20"/>
+      <c r="Y113" s="20"/>
+      <c r="Z113" s="20"/>
+      <c r="AA113" s="20"/>
+    </row>
+    <row r="114" spans="1:27">
+      <c r="E114" s="13"/>
+    </row>
+    <row r="115" spans="1:27" ht="23">
+      <c r="A115" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C105" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D105" s="24"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
-      <c r="H105" s="24"/>
-      <c r="I105" s="24"/>
-      <c r="J105" s="24"/>
-      <c r="K105" s="24"/>
-      <c r="L105" s="24"/>
-      <c r="M105" s="24"/>
-      <c r="N105" s="24"/>
-      <c r="O105" s="24"/>
-      <c r="P105" s="24"/>
-      <c r="Q105" s="24"/>
-      <c r="R105" s="24"/>
-      <c r="S105" s="24"/>
-      <c r="T105" s="24"/>
-      <c r="U105" s="24"/>
-      <c r="V105" s="24"/>
-      <c r="W105" s="24"/>
-      <c r="X105" s="24"/>
-      <c r="Y105" s="24"/>
-      <c r="Z105" s="24"/>
-      <c r="AA105" s="24"/>
-    </row>
-    <row r="106" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B106" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C106" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D106" s="24"/>
-      <c r="E106" s="15"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
-      <c r="H106" s="24"/>
-      <c r="I106" s="24"/>
-      <c r="J106" s="24"/>
-      <c r="K106" s="24"/>
-      <c r="L106" s="24"/>
-      <c r="M106" s="24"/>
-      <c r="N106" s="24"/>
-      <c r="O106" s="24"/>
-      <c r="P106" s="24"/>
-      <c r="Q106" s="24"/>
-      <c r="R106" s="24"/>
-      <c r="S106" s="24"/>
-      <c r="T106" s="24"/>
-      <c r="U106" s="24"/>
-      <c r="V106" s="24"/>
-      <c r="W106" s="24"/>
-      <c r="X106" s="24"/>
-      <c r="Y106" s="24"/>
-      <c r="Z106" s="24"/>
-      <c r="AA106" s="24"/>
-    </row>
-    <row r="107" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C107" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D107" s="24"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="24"/>
-      <c r="G107" s="24"/>
-      <c r="H107" s="24"/>
-      <c r="I107" s="24"/>
-      <c r="J107" s="24"/>
-      <c r="K107" s="24"/>
-      <c r="L107" s="24"/>
-      <c r="M107" s="24"/>
-      <c r="N107" s="24"/>
-      <c r="O107" s="24"/>
-      <c r="P107" s="24"/>
-      <c r="Q107" s="24"/>
-      <c r="R107" s="24"/>
-      <c r="S107" s="24"/>
-      <c r="T107" s="24"/>
-      <c r="U107" s="24"/>
-      <c r="V107" s="24"/>
-      <c r="W107" s="24"/>
-      <c r="X107" s="24"/>
-      <c r="Y107" s="24"/>
-      <c r="Z107" s="24"/>
-      <c r="AA107" s="24"/>
-    </row>
-    <row r="108" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C108" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D108" s="24"/>
-      <c r="E108" s="15"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
-      <c r="H108" s="24"/>
-      <c r="I108" s="24"/>
-      <c r="J108" s="24"/>
-      <c r="K108" s="24"/>
-      <c r="L108" s="24"/>
-      <c r="M108" s="24"/>
-      <c r="N108" s="24"/>
-      <c r="O108" s="24"/>
-      <c r="P108" s="24"/>
-      <c r="Q108" s="24"/>
-      <c r="R108" s="24"/>
-      <c r="S108" s="24"/>
-      <c r="T108" s="24"/>
-      <c r="U108" s="24"/>
-      <c r="V108" s="24"/>
-      <c r="W108" s="24"/>
-      <c r="X108" s="24"/>
-      <c r="Y108" s="24"/>
-      <c r="Z108" s="24"/>
-      <c r="AA108" s="24"/>
-    </row>
-    <row r="109" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C109" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D109" s="24"/>
-      <c r="E109" s="15"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
-      <c r="H109" s="24"/>
-      <c r="I109" s="24"/>
-      <c r="J109" s="24"/>
-      <c r="K109" s="24"/>
-      <c r="L109" s="24"/>
-      <c r="M109" s="24"/>
-      <c r="N109" s="24"/>
-      <c r="O109" s="24"/>
-      <c r="P109" s="24"/>
-      <c r="Q109" s="24"/>
-      <c r="R109" s="24"/>
-      <c r="S109" s="24"/>
-      <c r="T109" s="24"/>
-      <c r="U109" s="24"/>
-      <c r="V109" s="24"/>
-      <c r="W109" s="24"/>
-      <c r="X109" s="24"/>
-      <c r="Y109" s="24"/>
-      <c r="Z109" s="24"/>
-      <c r="AA109" s="24"/>
-    </row>
-    <row r="110" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C110" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D110" s="24"/>
-      <c r="E110" s="15"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="24"/>
-      <c r="H110" s="24"/>
-      <c r="I110" s="24"/>
-      <c r="J110" s="24"/>
-      <c r="K110" s="24"/>
-      <c r="L110" s="24"/>
-      <c r="M110" s="24"/>
-      <c r="N110" s="24"/>
-      <c r="O110" s="24"/>
-      <c r="P110" s="24"/>
-      <c r="Q110" s="24"/>
-      <c r="R110" s="24"/>
-      <c r="S110" s="24"/>
-      <c r="T110" s="24"/>
-      <c r="U110" s="24"/>
-      <c r="V110" s="24"/>
-      <c r="W110" s="24"/>
-      <c r="X110" s="24"/>
-      <c r="Y110" s="24"/>
-      <c r="Z110" s="24"/>
-      <c r="AA110" s="24"/>
-    </row>
-    <row r="111" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C111" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D111" s="24"/>
-      <c r="E111" s="15"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="24"/>
-      <c r="H111" s="24"/>
-      <c r="I111" s="24"/>
-      <c r="J111" s="24"/>
-      <c r="K111" s="24"/>
-      <c r="L111" s="24"/>
-      <c r="M111" s="24"/>
-      <c r="N111" s="24"/>
-      <c r="O111" s="24"/>
-      <c r="P111" s="24"/>
-      <c r="Q111" s="24"/>
-      <c r="R111" s="24"/>
-      <c r="S111" s="24"/>
-      <c r="T111" s="24"/>
-      <c r="U111" s="24"/>
-      <c r="V111" s="24"/>
-      <c r="W111" s="24"/>
-      <c r="X111" s="24"/>
-      <c r="Y111" s="24"/>
-      <c r="Z111" s="24"/>
-      <c r="AA111" s="24"/>
-    </row>
-    <row r="112" spans="1:27" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C112" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D112" s="24"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="30"/>
-      <c r="G112" s="24"/>
-      <c r="H112" s="24"/>
-      <c r="I112" s="24"/>
-      <c r="J112" s="24"/>
-      <c r="K112" s="24"/>
-      <c r="L112" s="24"/>
-      <c r="M112" s="24"/>
-      <c r="N112" s="24"/>
-      <c r="O112" s="24"/>
-      <c r="P112" s="24"/>
-      <c r="Q112" s="24"/>
-      <c r="R112" s="24"/>
-      <c r="S112" s="24"/>
-      <c r="T112" s="24"/>
-      <c r="U112" s="24"/>
-      <c r="V112" s="24"/>
-      <c r="W112" s="24"/>
-      <c r="X112" s="24"/>
-      <c r="Y112" s="24"/>
-      <c r="Z112" s="24"/>
-      <c r="AA112" s="24"/>
-    </row>
-    <row r="113" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C113" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D113" s="24"/>
-      <c r="E113" s="15"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="24"/>
-      <c r="H113" s="24"/>
-      <c r="I113" s="24"/>
-      <c r="J113" s="24"/>
-      <c r="K113" s="24"/>
-      <c r="L113" s="24"/>
-      <c r="M113" s="24"/>
-      <c r="N113" s="24"/>
-      <c r="O113" s="24"/>
-      <c r="P113" s="24"/>
-      <c r="Q113" s="24"/>
-      <c r="R113" s="24"/>
-      <c r="S113" s="24"/>
-      <c r="T113" s="24"/>
-      <c r="U113" s="24"/>
-      <c r="V113" s="24"/>
-      <c r="W113" s="24"/>
-      <c r="X113" s="24"/>
-      <c r="Y113" s="24"/>
-      <c r="Z113" s="24"/>
-      <c r="AA113" s="24"/>
-    </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E114" s="15"/>
-    </row>
-    <row r="115" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A115" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E115" s="15"/>
-    </row>
-    <row r="116" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
+      <c r="E115" s="13"/>
+    </row>
+    <row r="116" spans="1:27" s="3" customFormat="1" ht="15">
+      <c r="A116" s="13"/>
       <c r="B116" s="4" t="s">
         <v>1</v>
       </c>
@@ -2825,101 +2846,101 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
+    <row r="117" spans="1:27" s="22" customFormat="1" ht="15">
+      <c r="A117" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="20" t="s">
+      <c r="B117" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C117" s="21" t="s">
+      <c r="C117" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E117" s="22"/>
-    </row>
-    <row r="118" spans="1:27" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
+      <c r="E117" s="28"/>
+    </row>
+    <row r="118" spans="1:27" s="22" customFormat="1" ht="15">
+      <c r="A118" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="20" t="s">
+      <c r="B118" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C118" s="21" t="s">
+      <c r="C118" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E118" s="22"/>
-    </row>
-    <row r="119" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+      <c r="E118" s="28"/>
+    </row>
+    <row r="119" spans="1:27" s="22" customFormat="1" ht="15">
+      <c r="A119" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="B119" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C119" s="20" t="s">
+      <c r="C119" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E119" s="22"/>
-    </row>
-    <row r="120" spans="1:27" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
+      <c r="E119" s="28"/>
+    </row>
+    <row r="120" spans="1:27" s="20" customFormat="1" ht="42">
+      <c r="A120" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B120" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C120" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E120" s="28"/>
+    </row>
+    <row r="121" spans="1:27" s="20" customFormat="1" ht="56">
+      <c r="A121" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C121" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="E121" s="28"/>
+    </row>
+    <row r="122" spans="1:27" s="9" customFormat="1" ht="42">
+      <c r="A122" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E122" s="28"/>
+    </row>
+    <row r="123" spans="1:27" s="9" customFormat="1" ht="42">
+      <c r="A123" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C123" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E120" s="22"/>
-    </row>
-    <row r="121" spans="1:27" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E121" s="22"/>
-    </row>
-    <row r="122" spans="1:27" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E122" s="22"/>
-    </row>
-    <row r="123" spans="1:27" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E123" s="22"/>
-    </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="E124" s="15"/>
-    </row>
-    <row r="125" spans="1:27" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A125" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="E125" s="15"/>
-    </row>
-    <row r="126" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="15"/>
+      <c r="E123" s="28"/>
+    </row>
+    <row r="124" spans="1:27">
+      <c r="E124" s="13"/>
+    </row>
+    <row r="125" spans="1:27" ht="23">
+      <c r="A125" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E125" s="13"/>
+    </row>
+    <row r="126" spans="1:27" s="3" customFormat="1" ht="15">
+      <c r="A126" s="13"/>
       <c r="B126" s="4" t="s">
         <v>1</v>
       </c>
@@ -2931,129 +2952,134 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:27" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" s="15" customFormat="1" ht="15">
       <c r="A127" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C127" s="17" t="s">
+      <c r="C127" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E127" s="15"/>
-    </row>
-    <row r="128" spans="1:27" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E127" s="13"/>
+    </row>
+    <row r="128" spans="1:27" s="15" customFormat="1" ht="15">
       <c r="A128" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="16" t="s">
+      <c r="B128" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C128" s="17" t="s">
+      <c r="C128" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E128" s="15"/>
-    </row>
-    <row r="129" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E128" s="13"/>
+    </row>
+    <row r="129" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A129" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B129" s="16" t="s">
+      <c r="B129" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="16" t="s">
+      <c r="C129" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E129" s="15"/>
-    </row>
-    <row r="130" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E129" s="13"/>
+    </row>
+    <row r="130" spans="1:5" s="15" customFormat="1" ht="15">
       <c r="A130" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="16" t="s">
+      <c r="B130" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="16" t="s">
+      <c r="C130" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E130" s="15"/>
-    </row>
-    <row r="131" spans="1:5" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E130" s="13"/>
+    </row>
+    <row r="131" spans="1:5" s="15" customFormat="1" ht="42">
       <c r="A131" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B131" s="16" t="s">
+      <c r="B131" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C131" s="16" t="s">
+      <c r="C131" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E131" s="15"/>
-    </row>
-    <row r="132" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E131" s="13"/>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E132" s="15"/>
-    </row>
-    <row r="133" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E132" s="13"/>
+    </row>
+    <row r="133" spans="1:5" s="3" customFormat="1" ht="28">
       <c r="A133" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E133" s="15"/>
-    </row>
-    <row r="134" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="E133" s="13"/>
+    </row>
+    <row r="134" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A134" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E134" s="15"/>
-    </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E134" s="13"/>
+    </row>
+    <row r="135" spans="1:5" ht="28">
       <c r="A135" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E135" s="15"/>
-    </row>
-    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E135" s="13"/>
+    </row>
+    <row r="136" spans="1:5" ht="28">
       <c r="A136" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E136" s="15"/>
+        <v>107</v>
+      </c>
+      <c r="E136" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3065,43 +3091,48 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:2">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>41772</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:2">
+      <c r="A4" s="13">
         <v>1.2</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="24">
         <v>41773</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Timesheet and Weekly Report (Week 4 Summer)
Timesheet and Weekly Report for Week 4 of Summer Term
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20500" windowHeight="7640"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20505" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="DTP" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="117">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Modified By</t>
+  </si>
+  <si>
+    <t>Roger Tan</t>
   </si>
 </sst>
 </file>
@@ -842,7 +848,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -873,9 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1198,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1208,34 +1211,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="40.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="20">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:6" s="13" customFormat="1" ht="15">
+    <row r="2" spans="1:6" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1243,80 +1246,80 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="15" customFormat="1" ht="15">
+    <row r="3" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" s="15" customFormat="1" ht="42">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" s="5" customFormat="1" ht="20">
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="15">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
@@ -1328,103 +1331,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="15" customFormat="1" ht="15">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" s="15" customFormat="1" ht="42">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" s="15" customFormat="1" ht="28">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="28">
+      <c r="E16" s="12"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="20">
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A20" s="13"/>
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
@@ -1436,67 +1439,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="15" customFormat="1" ht="15">
+    <row r="21" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" s="15" customFormat="1" ht="42">
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1506,9 +1509,9 @@
       <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -1518,21 +1521,21 @@
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" customFormat="1">
-      <c r="A28" s="16"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="20">
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="11"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
       <c r="B30" s="4" t="s">
         <v>1</v>
       </c>
@@ -1544,67 +1547,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="15" customFormat="1" ht="15">
+    <row r="31" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:5" s="15" customFormat="1" ht="42">
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
@@ -1614,9 +1617,9 @@
       <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
@@ -1626,9 +1629,9 @@
       <c r="C37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="56">
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1638,20 +1641,20 @@
       <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1">
-      <c r="A39" s="13"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="20">
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A41" s="13"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
       <c r="B41" s="4" t="s">
         <v>1</v>
       </c>
@@ -1659,69 +1662,69 @@
         <v>0</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="1:5" s="15" customFormat="1" ht="42">
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1731,9 +1734,9 @@
       <c r="C47" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="13"/>
-    </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E47" s="12"/>
+    </row>
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
@@ -1743,9 +1746,9 @@
       <c r="C48" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="13"/>
-    </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E48" s="12"/>
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>9</v>
       </c>
@@ -1755,9 +1758,9 @@
       <c r="C49" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -1767,20 +1770,20 @@
       <c r="C50" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="13"/>
-    </row>
-    <row r="51" spans="1:5" s="3" customFormat="1">
-      <c r="A51" s="13"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="20">
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A53" s="13"/>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
       <c r="B53" s="4" t="s">
         <v>1</v>
       </c>
@@ -1792,67 +1795,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="15" customFormat="1" ht="15">
+    <row r="54" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="13"/>
-    </row>
-    <row r="55" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="13"/>
-    </row>
-    <row r="56" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="13"/>
-    </row>
-    <row r="58" spans="1:5" s="15" customFormat="1" ht="42">
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="13"/>
-    </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" ht="15">
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -1862,9 +1865,9 @@
       <c r="C59" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E59" s="13"/>
-    </row>
-    <row r="60" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -1874,9 +1877,9 @@
       <c r="C60" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="61" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="E60" s="12"/>
+    </row>
+    <row r="61" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>9</v>
       </c>
@@ -1886,19 +1889,19 @@
       <c r="C61" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="13"/>
-    </row>
-    <row r="62" spans="1:5" customFormat="1">
-      <c r="E62" s="13"/>
-    </row>
-    <row r="63" spans="1:5" s="9" customFormat="1" ht="23">
-      <c r="A63" s="17" t="s">
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="12"/>
+    </row>
+    <row r="63" spans="1:5" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E63" s="13"/>
-    </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="15">
-      <c r="A64" s="13"/>
+      <c r="E63" s="12"/>
+    </row>
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
       <c r="B64" s="4" t="s">
         <v>1</v>
       </c>
@@ -1906,69 +1909,69 @@
         <v>0</v>
       </c>
       <c r="D64" s="7"/>
-      <c r="E64" s="13"/>
-    </row>
-    <row r="65" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="13"/>
-    </row>
-    <row r="66" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="13"/>
-    </row>
-    <row r="69" spans="1:6" s="15" customFormat="1" ht="42">
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="13"/>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>7</v>
       </c>
@@ -1978,9 +1981,9 @@
       <c r="C70" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="13"/>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="28">
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -1990,9 +1993,9 @@
       <c r="C71" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E71" s="13"/>
-    </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="56">
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="1:6" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -2002,20 +2005,20 @@
       <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E72" s="13"/>
+      <c r="E72" s="12"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1">
-      <c r="E73" s="13"/>
-    </row>
-    <row r="74" spans="1:6" ht="23">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="12"/>
+    </row>
+    <row r="74" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E74" s="13"/>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="15">
-      <c r="A75" s="13"/>
+      <c r="E74" s="12"/>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="12"/>
       <c r="B75" s="4" t="s">
         <v>1</v>
       </c>
@@ -2027,67 +2030,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="15" customFormat="1" ht="15">
+    <row r="76" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="13"/>
-    </row>
-    <row r="77" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C77" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="13"/>
-    </row>
-    <row r="78" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E77" s="12"/>
+    </row>
+    <row r="78" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E78" s="13"/>
-    </row>
-    <row r="79" spans="1:6" s="15" customFormat="1" ht="15">
+      <c r="E78" s="12"/>
+    </row>
+    <row r="79" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E79" s="13"/>
-    </row>
-    <row r="80" spans="1:6" s="15" customFormat="1" ht="42">
+      <c r="E79" s="12"/>
+    </row>
+    <row r="80" spans="1:6" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E80" s="13"/>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="15">
+      <c r="E80" s="12"/>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>7</v>
       </c>
@@ -2097,9 +2100,9 @@
       <c r="C81" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E81" s="13"/>
-    </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="28">
+      <c r="E81" s="12"/>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
@@ -2109,9 +2112,9 @@
       <c r="C82" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E82" s="13"/>
-    </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="E82" s="12"/>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>9</v>
       </c>
@@ -2121,19 +2124,19 @@
       <c r="C83" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E83" s="13"/>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1">
-      <c r="E84" s="13"/>
-    </row>
-    <row r="85" spans="1:6" ht="23">
+      <c r="E83" s="12"/>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E84" s="12"/>
+    </row>
+    <row r="85" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A85" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E85" s="13"/>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="15">
-      <c r="A86" s="13"/>
+      <c r="E85" s="12"/>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="12"/>
       <c r="B86" s="4" t="s">
         <v>1</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1">
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>2</v>
       </c>
@@ -2155,9 +2158,9 @@
       <c r="C87" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="13"/>
-    </row>
-    <row r="88" spans="1:6" s="3" customFormat="1">
+      <c r="E87" s="12"/>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -2167,9 +2170,9 @@
       <c r="C88" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="13"/>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1">
+      <c r="E88" s="12"/>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>4</v>
       </c>
@@ -2179,9 +2182,9 @@
       <c r="C89" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E89" s="13"/>
-    </row>
-    <row r="90" spans="1:6" s="3" customFormat="1">
+      <c r="E89" s="12"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
@@ -2191,9 +2194,9 @@
       <c r="C90" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E90" s="13"/>
-    </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="E90" s="12"/>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>6</v>
       </c>
@@ -2203,9 +2206,9 @@
       <c r="C91" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E91" s="13"/>
-    </row>
-    <row r="92" spans="1:6" s="3" customFormat="1">
+      <c r="E91" s="12"/>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
@@ -2215,9 +2218,9 @@
       <c r="C92" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E92" s="13"/>
-    </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="28">
+      <c r="E92" s="12"/>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>7</v>
       </c>
@@ -2227,9 +2230,9 @@
       <c r="C93" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E93" s="13"/>
-    </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="E93" s="12"/>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>8</v>
       </c>
@@ -2239,20 +2242,20 @@
       <c r="C94" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E94" s="13"/>
+      <c r="E94" s="12"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" spans="1:6">
-      <c r="E95" s="13"/>
-    </row>
-    <row r="96" spans="1:6" ht="23">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="12"/>
+    </row>
+    <row r="96" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E96" s="13"/>
-    </row>
-    <row r="97" spans="1:27" s="3" customFormat="1" ht="15">
-      <c r="A97" s="13"/>
+      <c r="E96" s="12"/>
+    </row>
+    <row r="97" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="12"/>
       <c r="B97" s="4" t="s">
         <v>1</v>
       </c>
@@ -2264,577 +2267,577 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:27" s="18" customFormat="1" ht="15">
-      <c r="A98" s="19" t="s">
+    <row r="98" spans="1:27" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B98" s="21" t="s">
+      <c r="B98" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="22" t="s">
+      <c r="C98" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D98" s="22"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="22"/>
-      <c r="G98" s="22"/>
-      <c r="H98" s="22"/>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
-      <c r="K98" s="22"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="22"/>
-      <c r="N98" s="22"/>
-      <c r="O98" s="22"/>
-      <c r="P98" s="22"/>
-      <c r="Q98" s="22"/>
-      <c r="R98" s="22"/>
-      <c r="S98" s="22"/>
-      <c r="T98" s="22"/>
-      <c r="U98" s="22"/>
-      <c r="V98" s="22"/>
-      <c r="W98" s="22"/>
-      <c r="X98" s="22"/>
-      <c r="Y98" s="22"/>
-      <c r="Z98" s="22"/>
-      <c r="AA98" s="22"/>
-    </row>
-    <row r="99" spans="1:27" s="18" customFormat="1" ht="15">
-      <c r="A99" s="19" t="s">
+      <c r="D98" s="21"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="21"/>
+      <c r="N98" s="21"/>
+      <c r="O98" s="21"/>
+      <c r="P98" s="21"/>
+      <c r="Q98" s="21"/>
+      <c r="R98" s="21"/>
+      <c r="S98" s="21"/>
+      <c r="T98" s="21"/>
+      <c r="U98" s="21"/>
+      <c r="V98" s="21"/>
+      <c r="W98" s="21"/>
+      <c r="X98" s="21"/>
+      <c r="Y98" s="21"/>
+      <c r="Z98" s="21"/>
+      <c r="AA98" s="21"/>
+    </row>
+    <row r="99" spans="1:27" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C99" s="22" t="s">
+      <c r="C99" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="22"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
-      <c r="I99" s="22"/>
-      <c r="J99" s="22"/>
-      <c r="K99" s="22"/>
-      <c r="L99" s="22"/>
-      <c r="M99" s="22"/>
-      <c r="N99" s="22"/>
-      <c r="O99" s="22"/>
-      <c r="P99" s="22"/>
-      <c r="Q99" s="22"/>
-      <c r="R99" s="22"/>
-      <c r="S99" s="22"/>
-      <c r="T99" s="22"/>
-      <c r="U99" s="22"/>
-      <c r="V99" s="22"/>
-      <c r="W99" s="22"/>
-      <c r="X99" s="22"/>
-      <c r="Y99" s="22"/>
-      <c r="Z99" s="22"/>
-      <c r="AA99" s="22"/>
-    </row>
-    <row r="100" spans="1:27" s="18" customFormat="1" ht="15">
-      <c r="A100" s="19" t="s">
+      <c r="D99" s="21"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="21"/>
+      <c r="J99" s="21"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="21"/>
+      <c r="N99" s="21"/>
+      <c r="O99" s="21"/>
+      <c r="P99" s="21"/>
+      <c r="Q99" s="21"/>
+      <c r="R99" s="21"/>
+      <c r="S99" s="21"/>
+      <c r="T99" s="21"/>
+      <c r="U99" s="21"/>
+      <c r="V99" s="21"/>
+      <c r="W99" s="21"/>
+      <c r="X99" s="21"/>
+      <c r="Y99" s="21"/>
+      <c r="Z99" s="21"/>
+      <c r="AA99" s="21"/>
+    </row>
+    <row r="100" spans="1:27" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="21" t="s">
+      <c r="B100" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C100" s="21" t="s">
+      <c r="C100" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D100" s="22"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
-      <c r="H100" s="22"/>
-      <c r="I100" s="22"/>
-      <c r="J100" s="22"/>
-      <c r="K100" s="22"/>
-      <c r="L100" s="22"/>
-      <c r="M100" s="22"/>
-      <c r="N100" s="22"/>
-      <c r="O100" s="22"/>
-      <c r="P100" s="22"/>
-      <c r="Q100" s="22"/>
-      <c r="R100" s="22"/>
-      <c r="S100" s="22"/>
-      <c r="T100" s="22"/>
-      <c r="U100" s="22"/>
-      <c r="V100" s="22"/>
-      <c r="W100" s="22"/>
-      <c r="X100" s="22"/>
-      <c r="Y100" s="22"/>
-      <c r="Z100" s="22"/>
-      <c r="AA100" s="22"/>
-    </row>
-    <row r="101" spans="1:27" s="18" customFormat="1" ht="15">
-      <c r="A101" s="19" t="s">
+      <c r="D100" s="21"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="21"/>
+      <c r="O100" s="21"/>
+      <c r="P100" s="21"/>
+      <c r="Q100" s="21"/>
+      <c r="R100" s="21"/>
+      <c r="S100" s="21"/>
+      <c r="T100" s="21"/>
+      <c r="U100" s="21"/>
+      <c r="V100" s="21"/>
+      <c r="W100" s="21"/>
+      <c r="X100" s="21"/>
+      <c r="Y100" s="21"/>
+      <c r="Z100" s="21"/>
+      <c r="AA100" s="21"/>
+    </row>
+    <row r="101" spans="1:27" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B101" s="21" t="s">
+      <c r="B101" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="21" t="s">
+      <c r="C101" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D101" s="22"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="22"/>
-      <c r="G101" s="22"/>
-      <c r="H101" s="22"/>
-      <c r="I101" s="22"/>
-      <c r="J101" s="22"/>
-      <c r="K101" s="22"/>
-      <c r="L101" s="22"/>
-      <c r="M101" s="22"/>
-      <c r="N101" s="22"/>
-      <c r="O101" s="22"/>
-      <c r="P101" s="22"/>
-      <c r="Q101" s="22"/>
-      <c r="R101" s="22"/>
-      <c r="S101" s="22"/>
-      <c r="T101" s="22"/>
-      <c r="U101" s="22"/>
-      <c r="V101" s="22"/>
-      <c r="W101" s="22"/>
-      <c r="X101" s="22"/>
-      <c r="Y101" s="22"/>
-      <c r="Z101" s="22"/>
-      <c r="AA101" s="22"/>
-    </row>
-    <row r="102" spans="1:27" s="18" customFormat="1" ht="42">
-      <c r="A102" s="19" t="s">
+      <c r="D101" s="21"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
+      <c r="J101" s="21"/>
+      <c r="K101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="21"/>
+      <c r="O101" s="21"/>
+      <c r="P101" s="21"/>
+      <c r="Q101" s="21"/>
+      <c r="R101" s="21"/>
+      <c r="S101" s="21"/>
+      <c r="T101" s="21"/>
+      <c r="U101" s="21"/>
+      <c r="V101" s="21"/>
+      <c r="W101" s="21"/>
+      <c r="X101" s="21"/>
+      <c r="Y101" s="21"/>
+      <c r="Z101" s="21"/>
+      <c r="AA101" s="21"/>
+    </row>
+    <row r="102" spans="1:27" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="21" t="s">
+      <c r="B102" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C102" s="21" t="s">
+      <c r="C102" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D102" s="22"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="22"/>
-      <c r="G102" s="22"/>
-      <c r="H102" s="22"/>
-      <c r="I102" s="22"/>
-      <c r="J102" s="22"/>
-      <c r="K102" s="22"/>
-      <c r="L102" s="22"/>
-      <c r="M102" s="22"/>
-      <c r="N102" s="22"/>
-      <c r="O102" s="22"/>
-      <c r="P102" s="22"/>
-      <c r="Q102" s="22"/>
-      <c r="R102" s="22"/>
-      <c r="S102" s="22"/>
-      <c r="T102" s="22"/>
-      <c r="U102" s="22"/>
-      <c r="V102" s="22"/>
-      <c r="W102" s="22"/>
-      <c r="X102" s="22"/>
-      <c r="Y102" s="22"/>
-      <c r="Z102" s="22"/>
-      <c r="AA102" s="22"/>
-    </row>
-    <row r="103" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A103" s="19" t="s">
+      <c r="D102" s="21"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="21"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="21"/>
+      <c r="N102" s="21"/>
+      <c r="O102" s="21"/>
+      <c r="P102" s="21"/>
+      <c r="Q102" s="21"/>
+      <c r="R102" s="21"/>
+      <c r="S102" s="21"/>
+      <c r="T102" s="21"/>
+      <c r="U102" s="21"/>
+      <c r="V102" s="21"/>
+      <c r="W102" s="21"/>
+      <c r="X102" s="21"/>
+      <c r="Y102" s="21"/>
+      <c r="Z102" s="21"/>
+      <c r="AA102" s="21"/>
+    </row>
+    <row r="103" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C103" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D103" s="20"/>
-      <c r="E103" s="13"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="20"/>
-      <c r="H103" s="20"/>
-      <c r="I103" s="20"/>
-      <c r="J103" s="20"/>
-      <c r="K103" s="20"/>
-      <c r="L103" s="20"/>
-      <c r="M103" s="20"/>
-      <c r="N103" s="20"/>
-      <c r="O103" s="20"/>
-      <c r="P103" s="20"/>
-      <c r="Q103" s="20"/>
-      <c r="R103" s="20"/>
-      <c r="S103" s="20"/>
-      <c r="T103" s="20"/>
-      <c r="U103" s="20"/>
-      <c r="V103" s="20"/>
-      <c r="W103" s="20"/>
-      <c r="X103" s="20"/>
-      <c r="Y103" s="20"/>
-      <c r="Z103" s="20"/>
-      <c r="AA103" s="20"/>
-    </row>
-    <row r="104" spans="1:27" s="8" customFormat="1" ht="42">
-      <c r="A104" s="19" t="s">
+      <c r="D103" s="19"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="19"/>
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+      <c r="O103" s="19"/>
+      <c r="P103" s="19"/>
+      <c r="Q103" s="19"/>
+      <c r="R103" s="19"/>
+      <c r="S103" s="19"/>
+      <c r="T103" s="19"/>
+      <c r="U103" s="19"/>
+      <c r="V103" s="19"/>
+      <c r="W103" s="19"/>
+      <c r="X103" s="19"/>
+      <c r="Y103" s="19"/>
+      <c r="Z103" s="19"/>
+      <c r="AA103" s="19"/>
+    </row>
+    <row r="104" spans="1:27" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="C104" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D104" s="20"/>
-      <c r="E104" s="13"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="20"/>
-      <c r="I104" s="20"/>
-      <c r="J104" s="20"/>
-      <c r="K104" s="20"/>
-      <c r="L104" s="20"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="20"/>
-      <c r="O104" s="20"/>
-      <c r="P104" s="20"/>
-      <c r="Q104" s="20"/>
-      <c r="R104" s="20"/>
-      <c r="S104" s="20"/>
-      <c r="T104" s="20"/>
-      <c r="U104" s="20"/>
-      <c r="V104" s="20"/>
-      <c r="W104" s="20"/>
-      <c r="X104" s="20"/>
-      <c r="Y104" s="20"/>
-      <c r="Z104" s="20"/>
-      <c r="AA104" s="20"/>
-    </row>
-    <row r="105" spans="1:27" s="8" customFormat="1" ht="15">
-      <c r="A105" s="19" t="s">
+      <c r="D104" s="19"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="L104" s="19"/>
+      <c r="M104" s="19"/>
+      <c r="N104" s="19"/>
+      <c r="O104" s="19"/>
+      <c r="P104" s="19"/>
+      <c r="Q104" s="19"/>
+      <c r="R104" s="19"/>
+      <c r="S104" s="19"/>
+      <c r="T104" s="19"/>
+      <c r="U104" s="19"/>
+      <c r="V104" s="19"/>
+      <c r="W104" s="19"/>
+      <c r="X104" s="19"/>
+      <c r="Y104" s="19"/>
+      <c r="Z104" s="19"/>
+      <c r="AA104" s="19"/>
+    </row>
+    <row r="105" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B105" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D105" s="20"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="20"/>
-      <c r="I105" s="20"/>
-      <c r="J105" s="20"/>
-      <c r="K105" s="20"/>
-      <c r="L105" s="20"/>
-      <c r="M105" s="20"/>
-      <c r="N105" s="20"/>
-      <c r="O105" s="20"/>
-      <c r="P105" s="20"/>
-      <c r="Q105" s="20"/>
-      <c r="R105" s="20"/>
-      <c r="S105" s="20"/>
-      <c r="T105" s="20"/>
-      <c r="U105" s="20"/>
-      <c r="V105" s="20"/>
-      <c r="W105" s="20"/>
-      <c r="X105" s="20"/>
-      <c r="Y105" s="20"/>
-      <c r="Z105" s="20"/>
-      <c r="AA105" s="20"/>
-    </row>
-    <row r="106" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A106" s="19" t="s">
+      <c r="D105" s="19"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="19"/>
+      <c r="J105" s="19"/>
+      <c r="K105" s="19"/>
+      <c r="L105" s="19"/>
+      <c r="M105" s="19"/>
+      <c r="N105" s="19"/>
+      <c r="O105" s="19"/>
+      <c r="P105" s="19"/>
+      <c r="Q105" s="19"/>
+      <c r="R105" s="19"/>
+      <c r="S105" s="19"/>
+      <c r="T105" s="19"/>
+      <c r="U105" s="19"/>
+      <c r="V105" s="19"/>
+      <c r="W105" s="19"/>
+      <c r="X105" s="19"/>
+      <c r="Y105" s="19"/>
+      <c r="Z105" s="19"/>
+      <c r="AA105" s="19"/>
+    </row>
+    <row r="106" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D106" s="20"/>
-      <c r="E106" s="13"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="20"/>
-      <c r="I106" s="20"/>
-      <c r="J106" s="20"/>
-      <c r="K106" s="20"/>
-      <c r="L106" s="20"/>
-      <c r="M106" s="20"/>
-      <c r="N106" s="20"/>
-      <c r="O106" s="20"/>
-      <c r="P106" s="20"/>
-      <c r="Q106" s="20"/>
-      <c r="R106" s="20"/>
-      <c r="S106" s="20"/>
-      <c r="T106" s="20"/>
-      <c r="U106" s="20"/>
-      <c r="V106" s="20"/>
-      <c r="W106" s="20"/>
-      <c r="X106" s="20"/>
-      <c r="Y106" s="20"/>
-      <c r="Z106" s="20"/>
-      <c r="AA106" s="20"/>
-    </row>
-    <row r="107" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A107" s="19" t="s">
+      <c r="D106" s="19"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="L106" s="19"/>
+      <c r="M106" s="19"/>
+      <c r="N106" s="19"/>
+      <c r="O106" s="19"/>
+      <c r="P106" s="19"/>
+      <c r="Q106" s="19"/>
+      <c r="R106" s="19"/>
+      <c r="S106" s="19"/>
+      <c r="T106" s="19"/>
+      <c r="U106" s="19"/>
+      <c r="V106" s="19"/>
+      <c r="W106" s="19"/>
+      <c r="X106" s="19"/>
+      <c r="Y106" s="19"/>
+      <c r="Z106" s="19"/>
+      <c r="AA106" s="19"/>
+    </row>
+    <row r="107" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
         <v>74</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C107" s="20" t="s">
+      <c r="C107" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D107" s="20"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="20"/>
-      <c r="J107" s="20"/>
-      <c r="K107" s="20"/>
-      <c r="L107" s="20"/>
-      <c r="M107" s="20"/>
-      <c r="N107" s="20"/>
-      <c r="O107" s="20"/>
-      <c r="P107" s="20"/>
-      <c r="Q107" s="20"/>
-      <c r="R107" s="20"/>
-      <c r="S107" s="20"/>
-      <c r="T107" s="20"/>
-      <c r="U107" s="20"/>
-      <c r="V107" s="20"/>
-      <c r="W107" s="20"/>
-      <c r="X107" s="20"/>
-      <c r="Y107" s="20"/>
-      <c r="Z107" s="20"/>
-      <c r="AA107" s="20"/>
-    </row>
-    <row r="108" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A108" s="19" t="s">
+      <c r="D107" s="19"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+      <c r="P107" s="19"/>
+      <c r="Q107" s="19"/>
+      <c r="R107" s="19"/>
+      <c r="S107" s="19"/>
+      <c r="T107" s="19"/>
+      <c r="U107" s="19"/>
+      <c r="V107" s="19"/>
+      <c r="W107" s="19"/>
+      <c r="X107" s="19"/>
+      <c r="Y107" s="19"/>
+      <c r="Z107" s="19"/>
+      <c r="AA107" s="19"/>
+    </row>
+    <row r="108" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
         <v>76</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C108" s="20" t="s">
+      <c r="C108" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D108" s="20"/>
-      <c r="E108" s="13"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="20"/>
-      <c r="I108" s="20"/>
-      <c r="J108" s="20"/>
-      <c r="K108" s="20"/>
-      <c r="L108" s="20"/>
-      <c r="M108" s="20"/>
-      <c r="N108" s="20"/>
-      <c r="O108" s="20"/>
-      <c r="P108" s="20"/>
-      <c r="Q108" s="20"/>
-      <c r="R108" s="20"/>
-      <c r="S108" s="20"/>
-      <c r="T108" s="20"/>
-      <c r="U108" s="20"/>
-      <c r="V108" s="20"/>
-      <c r="W108" s="20"/>
-      <c r="X108" s="20"/>
-      <c r="Y108" s="20"/>
-      <c r="Z108" s="20"/>
-      <c r="AA108" s="20"/>
-    </row>
-    <row r="109" spans="1:27" s="8" customFormat="1" ht="15">
-      <c r="A109" s="19" t="s">
+      <c r="D108" s="19"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+      <c r="J108" s="19"/>
+      <c r="K108" s="19"/>
+      <c r="L108" s="19"/>
+      <c r="M108" s="19"/>
+      <c r="N108" s="19"/>
+      <c r="O108" s="19"/>
+      <c r="P108" s="19"/>
+      <c r="Q108" s="19"/>
+      <c r="R108" s="19"/>
+      <c r="S108" s="19"/>
+      <c r="T108" s="19"/>
+      <c r="U108" s="19"/>
+      <c r="V108" s="19"/>
+      <c r="W108" s="19"/>
+      <c r="X108" s="19"/>
+      <c r="Y108" s="19"/>
+      <c r="Z108" s="19"/>
+      <c r="AA108" s="19"/>
+    </row>
+    <row r="109" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C109" s="20" t="s">
+      <c r="C109" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D109" s="20"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="20"/>
-      <c r="I109" s="20"/>
-      <c r="J109" s="20"/>
-      <c r="K109" s="20"/>
-      <c r="L109" s="20"/>
-      <c r="M109" s="20"/>
-      <c r="N109" s="20"/>
-      <c r="O109" s="20"/>
-      <c r="P109" s="20"/>
-      <c r="Q109" s="20"/>
-      <c r="R109" s="20"/>
-      <c r="S109" s="20"/>
-      <c r="T109" s="20"/>
-      <c r="U109" s="20"/>
-      <c r="V109" s="20"/>
-      <c r="W109" s="20"/>
-      <c r="X109" s="20"/>
-      <c r="Y109" s="20"/>
-      <c r="Z109" s="20"/>
-      <c r="AA109" s="20"/>
-    </row>
-    <row r="110" spans="1:27" s="8" customFormat="1" ht="15">
-      <c r="A110" s="19" t="s">
+      <c r="D109" s="19"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+      <c r="J109" s="19"/>
+      <c r="K109" s="19"/>
+      <c r="L109" s="19"/>
+      <c r="M109" s="19"/>
+      <c r="N109" s="19"/>
+      <c r="O109" s="19"/>
+      <c r="P109" s="19"/>
+      <c r="Q109" s="19"/>
+      <c r="R109" s="19"/>
+      <c r="S109" s="19"/>
+      <c r="T109" s="19"/>
+      <c r="U109" s="19"/>
+      <c r="V109" s="19"/>
+      <c r="W109" s="19"/>
+      <c r="X109" s="19"/>
+      <c r="Y109" s="19"/>
+      <c r="Z109" s="19"/>
+      <c r="AA109" s="19"/>
+    </row>
+    <row r="110" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="18" t="s">
         <v>81</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="20" t="s">
+      <c r="C110" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D110" s="20"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-      <c r="J110" s="20"/>
-      <c r="K110" s="20"/>
-      <c r="L110" s="20"/>
-      <c r="M110" s="20"/>
-      <c r="N110" s="20"/>
-      <c r="O110" s="20"/>
-      <c r="P110" s="20"/>
-      <c r="Q110" s="20"/>
-      <c r="R110" s="20"/>
-      <c r="S110" s="20"/>
-      <c r="T110" s="20"/>
-      <c r="U110" s="20"/>
-      <c r="V110" s="20"/>
-      <c r="W110" s="20"/>
-      <c r="X110" s="20"/>
-      <c r="Y110" s="20"/>
-      <c r="Z110" s="20"/>
-      <c r="AA110" s="20"/>
-    </row>
-    <row r="111" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A111" s="19" t="s">
+      <c r="D110" s="19"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
+      <c r="J110" s="19"/>
+      <c r="K110" s="19"/>
+      <c r="L110" s="19"/>
+      <c r="M110" s="19"/>
+      <c r="N110" s="19"/>
+      <c r="O110" s="19"/>
+      <c r="P110" s="19"/>
+      <c r="Q110" s="19"/>
+      <c r="R110" s="19"/>
+      <c r="S110" s="19"/>
+      <c r="T110" s="19"/>
+      <c r="U110" s="19"/>
+      <c r="V110" s="19"/>
+      <c r="W110" s="19"/>
+      <c r="X110" s="19"/>
+      <c r="Y110" s="19"/>
+      <c r="Z110" s="19"/>
+      <c r="AA110" s="19"/>
+    </row>
+    <row r="111" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
         <v>84</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D111" s="20"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
-      <c r="J111" s="20"/>
-      <c r="K111" s="20"/>
-      <c r="L111" s="20"/>
-      <c r="M111" s="20"/>
-      <c r="N111" s="20"/>
-      <c r="O111" s="20"/>
-      <c r="P111" s="20"/>
-      <c r="Q111" s="20"/>
-      <c r="R111" s="20"/>
-      <c r="S111" s="20"/>
-      <c r="T111" s="20"/>
-      <c r="U111" s="20"/>
-      <c r="V111" s="20"/>
-      <c r="W111" s="20"/>
-      <c r="X111" s="20"/>
-      <c r="Y111" s="20"/>
-      <c r="Z111" s="20"/>
-      <c r="AA111" s="20"/>
-    </row>
-    <row r="112" spans="1:27" s="8" customFormat="1" ht="28">
-      <c r="A112" s="19" t="s">
+      <c r="D111" s="19"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="19"/>
+      <c r="I111" s="19"/>
+      <c r="J111" s="19"/>
+      <c r="K111" s="19"/>
+      <c r="L111" s="19"/>
+      <c r="M111" s="19"/>
+      <c r="N111" s="19"/>
+      <c r="O111" s="19"/>
+      <c r="P111" s="19"/>
+      <c r="Q111" s="19"/>
+      <c r="R111" s="19"/>
+      <c r="S111" s="19"/>
+      <c r="T111" s="19"/>
+      <c r="U111" s="19"/>
+      <c r="V111" s="19"/>
+      <c r="W111" s="19"/>
+      <c r="X111" s="19"/>
+      <c r="Y111" s="19"/>
+      <c r="Z111" s="19"/>
+      <c r="AA111" s="19"/>
+    </row>
+    <row r="112" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="C112" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D112" s="20"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="26"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="20"/>
-      <c r="I112" s="20"/>
-      <c r="J112" s="20"/>
-      <c r="K112" s="20"/>
-      <c r="L112" s="20"/>
-      <c r="M112" s="20"/>
-      <c r="N112" s="20"/>
-      <c r="O112" s="20"/>
-      <c r="P112" s="20"/>
-      <c r="Q112" s="20"/>
-      <c r="R112" s="20"/>
-      <c r="S112" s="20"/>
-      <c r="T112" s="20"/>
-      <c r="U112" s="20"/>
-      <c r="V112" s="20"/>
-      <c r="W112" s="20"/>
-      <c r="X112" s="20"/>
-      <c r="Y112" s="20"/>
-      <c r="Z112" s="20"/>
-      <c r="AA112" s="20"/>
-    </row>
-    <row r="113" spans="1:27" s="8" customFormat="1" ht="15">
-      <c r="A113" s="19" t="s">
+      <c r="D112" s="19"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="19"/>
+      <c r="L112" s="19"/>
+      <c r="M112" s="19"/>
+      <c r="N112" s="19"/>
+      <c r="O112" s="19"/>
+      <c r="P112" s="19"/>
+      <c r="Q112" s="19"/>
+      <c r="R112" s="19"/>
+      <c r="S112" s="19"/>
+      <c r="T112" s="19"/>
+      <c r="U112" s="19"/>
+      <c r="V112" s="19"/>
+      <c r="W112" s="19"/>
+      <c r="X112" s="19"/>
+      <c r="Y112" s="19"/>
+      <c r="Z112" s="19"/>
+      <c r="AA112" s="19"/>
+    </row>
+    <row r="113" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B113" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C113" s="20" t="s">
+      <c r="C113" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D113" s="20"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
-      <c r="J113" s="20"/>
-      <c r="K113" s="20"/>
-      <c r="L113" s="20"/>
-      <c r="M113" s="20"/>
-      <c r="N113" s="20"/>
-      <c r="O113" s="20"/>
-      <c r="P113" s="20"/>
-      <c r="Q113" s="20"/>
-      <c r="R113" s="20"/>
-      <c r="S113" s="20"/>
-      <c r="T113" s="20"/>
-      <c r="U113" s="20"/>
-      <c r="V113" s="20"/>
-      <c r="W113" s="20"/>
-      <c r="X113" s="20"/>
-      <c r="Y113" s="20"/>
-      <c r="Z113" s="20"/>
-      <c r="AA113" s="20"/>
-    </row>
-    <row r="114" spans="1:27">
-      <c r="E114" s="13"/>
-    </row>
-    <row r="115" spans="1:27" ht="23">
+      <c r="D113" s="19"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
+      <c r="J113" s="19"/>
+      <c r="K113" s="19"/>
+      <c r="L113" s="19"/>
+      <c r="M113" s="19"/>
+      <c r="N113" s="19"/>
+      <c r="O113" s="19"/>
+      <c r="P113" s="19"/>
+      <c r="Q113" s="19"/>
+      <c r="R113" s="19"/>
+      <c r="S113" s="19"/>
+      <c r="T113" s="19"/>
+      <c r="U113" s="19"/>
+      <c r="V113" s="19"/>
+      <c r="W113" s="19"/>
+      <c r="X113" s="19"/>
+      <c r="Y113" s="19"/>
+      <c r="Z113" s="19"/>
+      <c r="AA113" s="19"/>
+    </row>
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E114" s="12"/>
+    </row>
+    <row r="115" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E115" s="13"/>
-    </row>
-    <row r="116" spans="1:27" s="3" customFormat="1" ht="15">
-      <c r="A116" s="13"/>
+      <c r="E115" s="12"/>
+    </row>
+    <row r="116" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="12"/>
       <c r="B116" s="4" t="s">
         <v>1</v>
       </c>
@@ -2846,56 +2849,56 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:27" s="22" customFormat="1" ht="15">
-      <c r="A117" s="19" t="s">
+    <row r="117" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="21" t="s">
+      <c r="B117" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C117" s="22" t="s">
+      <c r="C117" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E117" s="28"/>
-    </row>
-    <row r="118" spans="1:27" s="22" customFormat="1" ht="15">
-      <c r="A118" s="19" t="s">
+      <c r="E117" s="27"/>
+    </row>
+    <row r="118" spans="1:27" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="21" t="s">
+      <c r="B118" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C118" s="22" t="s">
+      <c r="C118" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E118" s="28"/>
-    </row>
-    <row r="119" spans="1:27" s="22" customFormat="1" ht="15">
-      <c r="A119" s="19" t="s">
+      <c r="E118" s="27"/>
+    </row>
+    <row r="119" spans="1:27" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B119" s="21" t="s">
+      <c r="B119" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C119" s="21" t="s">
+      <c r="C119" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E119" s="28"/>
-    </row>
-    <row r="120" spans="1:27" s="20" customFormat="1" ht="42">
-      <c r="A120" s="19" t="s">
+      <c r="E119" s="27"/>
+    </row>
+    <row r="120" spans="1:27" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B120" s="20" t="s">
+      <c r="B120" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C120" s="20" t="s">
+      <c r="C120" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E120" s="28"/>
-    </row>
-    <row r="121" spans="1:27" s="20" customFormat="1" ht="56">
-      <c r="A121" s="19" t="s">
+      <c r="E120" s="27"/>
+    </row>
+    <row r="121" spans="1:27" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A121" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B121" s="9" t="s">
@@ -2904,10 +2907,10 @@
       <c r="C121" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E121" s="28"/>
-    </row>
-    <row r="122" spans="1:27" s="9" customFormat="1" ht="42">
-      <c r="A122" s="19" t="s">
+      <c r="E121" s="27"/>
+    </row>
+    <row r="122" spans="1:27" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B122" s="9" t="s">
@@ -2916,10 +2919,10 @@
       <c r="C122" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E122" s="28"/>
-    </row>
-    <row r="123" spans="1:27" s="9" customFormat="1" ht="42">
-      <c r="A123" s="19" t="s">
+      <c r="E122" s="27"/>
+    </row>
+    <row r="123" spans="1:27" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B123" s="9" t="s">
@@ -2928,19 +2931,19 @@
       <c r="C123" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E123" s="28"/>
-    </row>
-    <row r="124" spans="1:27">
-      <c r="E124" s="13"/>
-    </row>
-    <row r="125" spans="1:27" ht="23">
-      <c r="A125" s="27" t="s">
+      <c r="E123" s="27"/>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E124" s="12"/>
+    </row>
+    <row r="125" spans="1:27" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A125" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="E125" s="13"/>
-    </row>
-    <row r="126" spans="1:27" s="3" customFormat="1" ht="15">
-      <c r="A126" s="13"/>
+      <c r="E125" s="12"/>
+    </row>
+    <row r="126" spans="1:27" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="12"/>
       <c r="B126" s="4" t="s">
         <v>1</v>
       </c>
@@ -2952,67 +2955,67 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:27" s="15" customFormat="1" ht="15">
+    <row r="127" spans="1:27" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="B127" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C127" s="15" t="s">
+      <c r="C127" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E127" s="13"/>
-    </row>
-    <row r="128" spans="1:27" s="15" customFormat="1" ht="15">
+      <c r="E127" s="12"/>
+    </row>
+    <row r="128" spans="1:27" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="B128" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C128" s="15" t="s">
+      <c r="C128" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E128" s="13"/>
-    </row>
-    <row r="129" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E128" s="12"/>
+    </row>
+    <row r="129" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C129" s="14" t="s">
+      <c r="C129" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E129" s="13"/>
-    </row>
-    <row r="130" spans="1:5" s="15" customFormat="1" ht="15">
+      <c r="E129" s="12"/>
+    </row>
+    <row r="130" spans="1:5" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="14" t="s">
+      <c r="C130" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E130" s="13"/>
-    </row>
-    <row r="131" spans="1:5" s="15" customFormat="1" ht="42">
+      <c r="E130" s="12"/>
+    </row>
+    <row r="131" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C131" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E131" s="13"/>
-    </row>
-    <row r="132" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E131" s="12"/>
+    </row>
+    <row r="132" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>7</v>
       </c>
@@ -3022,9 +3025,9 @@
       <c r="C132" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E132" s="13"/>
-    </row>
-    <row r="133" spans="1:5" s="3" customFormat="1" ht="28">
+      <c r="E132" s="12"/>
+    </row>
+    <row r="133" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>8</v>
       </c>
@@ -3034,9 +3037,9 @@
       <c r="C133" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E133" s="13"/>
-    </row>
-    <row r="134" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="E133" s="12"/>
+    </row>
+    <row r="134" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>9</v>
       </c>
@@ -3046,9 +3049,9 @@
       <c r="C134" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E134" s="13"/>
-    </row>
-    <row r="135" spans="1:5" ht="28">
+      <c r="E134" s="12"/>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>18</v>
       </c>
@@ -3058,9 +3061,9 @@
       <c r="C135" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E135" s="13"/>
-    </row>
-    <row r="136" spans="1:5" ht="28">
+      <c r="E135" s="12"/>
+    </row>
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>74</v>
       </c>
@@ -3070,7 +3073,7 @@
       <c r="C136" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E136" s="13"/>
+      <c r="E136" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3085,46 +3088,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="23">
         <v>41772</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="13">
+      <c r="C3" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>1.2</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>41773</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed minor bug with the slideshow. Updated DTP records
Fixed minor bug with the slideshow. It is reflected in Jira.
Fixed the scene.setfill issue as well. It was throwing exception that it
was null.
Updated the DTP records as well.
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="160">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -194,211 +194,7 @@
     <t>A fullscreen slide which displays images appears</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Click on the "Next" Button or press the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrow key </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>thrice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to advance to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fourth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> slide</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click on the "Next" Button or press the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrow key </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>twice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to advance to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>third</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> slide</t>
-    </r>
-  </si>
-  <si>
     <t>A fullscreen slide which play audios appears</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Click on the "Next" Button or press the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrow key </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">four </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">times to advance to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fifth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> slide</t>
-    </r>
   </si>
   <si>
     <t>A fullscreen slide which play videos appears</t>
@@ -468,74 +264,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Click on the "Next" Button or press the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Right</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arrow key </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>once</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to advance to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>second</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> slide</t>
-    </r>
-  </si>
-  <si>
     <t>Scroll to the Shape section inside the Playlist</t>
   </si>
   <si>
@@ -833,6 +561,239 @@
   </si>
   <si>
     <t>The fullscreen main menu window is closed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the "Next" Button or press the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrow key till you advance to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fourth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> slide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the "Next" Button or press the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrow key till you advance to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>third</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> slide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the "Next" Button or press the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrow key till you advance to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fifth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> slide</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on the "Next" Button or press the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arrow key till you advance to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>second</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> slide</t>
+    </r>
+  </si>
+  <si>
+    <t>Load External Recipe</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Document created</t>
+  </si>
+  <si>
+    <t>Redefine the instruction for each step</t>
+  </si>
+  <si>
+    <t>Slightly redefine the instruction for opening up a Playlist</t>
+  </si>
+  <si>
+    <t>Added more User Stories Tests</t>
+  </si>
+  <si>
+    <t>Click on the "Load External Recipe" Button</t>
+  </si>
+  <si>
+    <t>A small window contain two Buttons pops up</t>
+  </si>
+  <si>
+    <t>A fullscreen slideshow based on the playlist appears</t>
+  </si>
+  <si>
+    <t>Press the ESC Key or the "Exit Slide" Button</t>
+  </si>
+  <si>
+    <t>The fullscreen slideshow is now closed and returns to the main menu window</t>
+  </si>
+  <si>
+    <t>Same result as step 4</t>
+  </si>
+  <si>
+    <t>Repeat step 4</t>
+  </si>
+  <si>
+    <t>Click on the "Browse" Button and navigate to the directary of the wanted Playlist</t>
+  </si>
+  <si>
+    <t>Click on the "HTTP" Button and insert the URL of the wanted Playlist</t>
   </si>
 </sst>
 </file>
@@ -932,7 +893,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1016,6 +977,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1291,7 +1273,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1299,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA161"/>
+  <dimension ref="A1:AA176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E1" s="11"/>
     </row>
@@ -1333,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1377,10 +1359,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E6" s="12"/>
     </row>
@@ -1389,10 +1371,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E7" s="12"/>
     </row>
@@ -1401,7 +1383,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>37</v>
@@ -1474,10 +1456,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -1486,10 +1468,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -1498,7 +1480,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>37</v>
@@ -1523,7 +1505,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>13</v>
@@ -1594,10 +1576,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E26" s="12"/>
     </row>
@@ -1606,10 +1588,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E27" s="12"/>
     </row>
@@ -1618,7 +1600,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>37</v>
@@ -1630,7 +1612,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>39</v>
@@ -1702,10 +1684,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E36" s="12"/>
     </row>
@@ -1714,10 +1696,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E37" s="12"/>
     </row>
@@ -1726,7 +1708,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>37</v>
@@ -1738,7 +1720,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>40</v>
@@ -1750,7 +1732,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>38</v>
@@ -1819,10 +1801,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E47" s="12"/>
     </row>
@@ -1831,10 +1813,10 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E48" s="12"/>
     </row>
@@ -1950,10 +1932,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E59" s="12"/>
     </row>
@@ -1962,10 +1944,10 @@
         <v>6</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E60" s="12"/>
     </row>
@@ -1974,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>37</v>
@@ -1986,10 +1968,10 @@
         <v>8</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E62" s="12"/>
     </row>
@@ -1998,10 +1980,10 @@
         <v>9</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E63" s="12"/>
     </row>
@@ -2066,10 +2048,10 @@
         <v>5</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E70" s="12"/>
     </row>
@@ -2078,10 +2060,10 @@
         <v>6</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E71" s="12"/>
     </row>
@@ -2090,7 +2072,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>37</v>
@@ -2102,10 +2084,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E73" s="12"/>
     </row>
@@ -2114,10 +2096,10 @@
         <v>9</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="5"/>
@@ -2185,10 +2167,10 @@
         <v>5</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E81" s="12"/>
     </row>
@@ -2197,10 +2179,10 @@
         <v>6</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E82" s="12"/>
     </row>
@@ -2209,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>37</v>
@@ -2221,10 +2203,10 @@
         <v>8</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E84" s="12"/>
     </row>
@@ -2233,10 +2215,10 @@
         <v>9</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E85" s="12"/>
     </row>
@@ -2303,10 +2285,10 @@
         <v>5</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E92" s="12"/>
     </row>
@@ -2315,10 +2297,10 @@
         <v>6</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E93" s="12"/>
     </row>
@@ -2327,7 +2309,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>37</v>
@@ -2339,10 +2321,10 @@
         <v>8</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E95" s="12"/>
     </row>
@@ -2351,10 +2333,10 @@
         <v>9</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E96" s="12"/>
       <c r="F96" s="5"/>
@@ -2364,7 +2346,7 @@
     </row>
     <row r="98" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E98" s="12"/>
     </row>
@@ -2491,10 +2473,10 @@
         <v>5</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E103" s="12"/>
     </row>
@@ -2503,10 +2485,10 @@
         <v>6</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E104" s="12"/>
     </row>
@@ -2515,10 +2497,10 @@
         <v>7</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D105" s="19"/>
       <c r="E105" s="12"/>
@@ -2550,10 +2532,10 @@
         <v>8</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D106" s="19"/>
       <c r="E106" s="12"/>
@@ -2585,10 +2567,10 @@
         <v>9</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D107" s="19"/>
       <c r="E107" s="12"/>
@@ -2620,10 +2602,10 @@
         <v>18</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D108" s="19"/>
       <c r="E108" s="12"/>
@@ -2652,13 +2634,13 @@
     </row>
     <row r="109" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D109" s="19"/>
       <c r="E109" s="12"/>
@@ -2687,13 +2669,13 @@
     </row>
     <row r="110" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D110" s="19"/>
       <c r="E110" s="12"/>
@@ -2722,13 +2704,13 @@
     </row>
     <row r="111" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D111" s="19"/>
       <c r="E111" s="12"/>
@@ -2757,13 +2739,13 @@
     </row>
     <row r="112" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D112" s="19"/>
       <c r="E112" s="12"/>
@@ -2792,13 +2774,13 @@
     </row>
     <row r="113" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D113" s="19"/>
       <c r="E113" s="12"/>
@@ -2827,13 +2809,13 @@
     </row>
     <row r="114" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D114" s="19"/>
       <c r="E114" s="12"/>
@@ -2862,13 +2844,13 @@
     </row>
     <row r="115" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D115" s="19"/>
       <c r="E115" s="12"/>
@@ -2900,7 +2882,7 @@
     </row>
     <row r="117" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E117" s="12"/>
     </row>
@@ -2958,10 +2940,10 @@
         <v>5</v>
       </c>
       <c r="B122" s="29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E122" s="27"/>
     </row>
@@ -2970,10 +2952,10 @@
         <v>6</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E123" s="27"/>
     </row>
@@ -2982,10 +2964,10 @@
         <v>7</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E124" s="27"/>
     </row>
@@ -2994,10 +2976,10 @@
         <v>8</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E125" s="27"/>
     </row>
@@ -3006,10 +2988,10 @@
         <v>9</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E126" s="27"/>
     </row>
@@ -3018,70 +3000,70 @@
         <v>18</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E127" s="27"/>
     </row>
     <row r="128" spans="1:27" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B128" s="21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E128" s="27"/>
     </row>
     <row r="129" spans="1:5" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E129" s="27"/>
     </row>
     <row r="130" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E130" s="27"/>
     </row>
     <row r="131" spans="1:5" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E131" s="27"/>
     </row>
     <row r="132" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B132" s="21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E132" s="27"/>
     </row>
@@ -3090,7 +3072,7 @@
     </row>
     <row r="134" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A134" s="26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E134" s="12"/>
     </row>
@@ -3148,10 +3130,10 @@
         <v>5</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E139" s="12"/>
     </row>
@@ -3160,10 +3142,10 @@
         <v>6</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E140" s="12"/>
     </row>
@@ -3172,10 +3154,10 @@
         <v>7</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E141" s="12"/>
     </row>
@@ -3184,10 +3166,10 @@
         <v>8</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E142" s="12"/>
     </row>
@@ -3196,10 +3178,10 @@
         <v>9</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E143" s="12"/>
     </row>
@@ -3208,28 +3190,28 @@
         <v>18</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E144" s="12"/>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E145" s="12"/>
     </row>
     <row r="147" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E147" s="12"/>
     </row>
@@ -3287,10 +3269,10 @@
         <v>5</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3298,10 +3280,10 @@
         <v>6</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3309,10 +3291,10 @@
         <v>7</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3320,10 +3302,10 @@
         <v>8</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3331,10 +3313,10 @@
         <v>9</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3342,55 +3324,178 @@
         <v>18</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A163" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E163" s="32"/>
+    </row>
+    <row r="164" spans="1:5" s="35" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="32"/>
+      <c r="B164" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="34"/>
+      <c r="E164" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E165" s="32"/>
+    </row>
+    <row r="166" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C166" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E166" s="32"/>
+    </row>
+    <row r="167" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A167" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C167" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E167" s="32"/>
+    </row>
+    <row r="168" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C168" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B169" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C169" s="35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B170" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C170" s="35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B171" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C171" s="35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C172" s="35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B174" s="3"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B175" s="3"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3405,10 +3510,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3416,9 +3521,10 @@
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>35</v>
       </c>
@@ -3426,16 +3532,27 @@
         <v>36</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="23">
+        <v>41685</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1.1000000000000001</v>
       </c>
@@ -3443,10 +3560,13 @@
         <v>41772</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1.2</v>
       </c>
@@ -3454,10 +3574,13 @@
         <v>41773</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>1.3</v>
       </c>
@@ -3465,10 +3588,13 @@
         <v>41781</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1.4</v>
       </c>
@@ -3476,7 +3602,10 @@
         <v>41784</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to FileHandler and LoadExternal Recipe Class
Changes made to FileHandler class openFile method. So that when the Get
recipes from local directory is pressed, the filebrowser will open
infront of the popped up window.  And prevents it from opening more
filebrowser when the button is clicked more than once. DTP records is
updated as well.
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20505" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20505" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DTP" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="180">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -91,13 +91,7 @@
     <t>Move Between Slide</t>
   </si>
   <si>
-    <t>Click on the "Next" Button</t>
-  </si>
-  <si>
     <t>Subsequent Slide will be displayed unless it is at the last slide</t>
-  </si>
-  <si>
-    <t>Click on the "Previous" Button</t>
   </si>
   <si>
     <t>Previous Slide will be displayed unless it is at the first slide</t>
@@ -302,15 +296,6 @@
     <t>Timer</t>
   </si>
   <si>
-    <t>Click on the "Play" Button on the Control Panel</t>
-  </si>
-  <si>
-    <t>Click on the "Pause" Button on the Control Panel</t>
-  </si>
-  <si>
-    <t>Repeat steps 1-6. Press the "Exit Slide" button on the Slide's Control Panel</t>
-  </si>
-  <si>
     <t>Subsequent content will be displayed onto the Slide after the current slide's duration has passed.</t>
   </si>
   <si>
@@ -344,9 +329,6 @@
     <t>Step 12</t>
   </si>
   <si>
-    <t>Click the Create timer button</t>
-  </si>
-  <si>
     <t>A second timer is created</t>
   </si>
   <si>
@@ -371,9 +353,6 @@
     <t>Step 16</t>
   </si>
   <si>
-    <t>Click on the Create Timer Button</t>
-  </si>
-  <si>
     <t>The digital timer starts counting down based on the duration set. Start button changes to pause After the duration has passed, a beep sound is produced.</t>
   </si>
   <si>
@@ -386,12 +365,6 @@
     <t>Click the "Pause" Button</t>
   </si>
   <si>
-    <t>Click the "Next Slide" Button</t>
-  </si>
-  <si>
-    <t>Click the "Previous Slide" Button</t>
-  </si>
-  <si>
     <t>Timers reset to the timer that was originally selected</t>
   </si>
   <si>
@@ -413,19 +386,7 @@
     <t>Re-slide the notes panel. The notes panel should display what you have keyed in earlier on.</t>
   </si>
   <si>
-    <t>Navigate to the "Code" folder. Open up the eCook folder and search for "0_notes".txt file. Double click on the .txt file.</t>
-  </si>
-  <si>
-    <t>The .txt file should display what you have keyed into the notes panel.</t>
-  </si>
-  <si>
-    <t>Return to the Slideshow and Click on the "Next Slide" Button</t>
-  </si>
-  <si>
     <t>A fullscreen slide window displaying shapes appears</t>
-  </si>
-  <si>
-    <t>Repeat steps 6-8. However, this time, search for "1_notes".txt file.</t>
   </si>
   <si>
     <t>The .txt file should display what you have keyed into the notes panel in slide "1".</t>
@@ -772,28 +733,127 @@
     <t>Click on the "Load External Recipe" Button</t>
   </si>
   <si>
-    <t>A small window contain two Buttons pops up</t>
-  </si>
-  <si>
-    <t>A fullscreen slideshow based on the playlist appears</t>
-  </si>
-  <si>
-    <t>Press the ESC Key or the "Exit Slide" Button</t>
-  </si>
-  <si>
-    <t>The fullscreen slideshow is now closed and returns to the main menu window</t>
-  </si>
-  <si>
-    <t>Same result as step 4</t>
-  </si>
-  <si>
-    <t>Repeat step 4</t>
-  </si>
-  <si>
-    <t>Click on the "Browse" Button and navigate to the directary of the wanted Playlist</t>
-  </si>
-  <si>
-    <t>Click on the "HTTP" Button and insert the URL of the wanted Playlist</t>
+    <t xml:space="preserve">Click on the "Download Recipes from eCook Store" Button </t>
+  </si>
+  <si>
+    <t>Navigate to eCook's defaultRecipes folder and ensure that there's isnt any recipes of example 1-3</t>
+  </si>
+  <si>
+    <t>A list of XML playlist inside the folder</t>
+  </si>
+  <si>
+    <t>A list of  recipes available to download appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select one of the example playlist and click on the "Download Selected Recipes" Button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to eCook's defaultRecipes folder </t>
+  </si>
+  <si>
+    <t>Now the selected playlist to be downloaded earlier on, will appear in the folder</t>
+  </si>
+  <si>
+    <t>In the Main Menu window, click on the "Recipes" Button</t>
+  </si>
+  <si>
+    <t>The downloaded recipes playlist is now reflected in the list of playable recipes</t>
+  </si>
+  <si>
+    <t>It returns to Main Menu now</t>
+  </si>
+  <si>
+    <t>Return to Main Menu window by clicking on the "Close" Button located at the top right hand corner</t>
+  </si>
+  <si>
+    <t>Main Menu window appears</t>
+  </si>
+  <si>
+    <t>Repeat step 5</t>
+  </si>
+  <si>
+    <t>Same result as step 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the "Get Recipes from Local Directory" Button </t>
+  </si>
+  <si>
+    <t>A filebrowser window pops up</t>
+  </si>
+  <si>
+    <t>Navigate to eCook's Resources folder and select one of the XML Playlist</t>
+  </si>
+  <si>
+    <t>The recently uploaded recipes playlist from local directory is now reflected in the list of playable recipes</t>
+  </si>
+  <si>
+    <t>Repeat step 10</t>
+  </si>
+  <si>
+    <t>Same result as step 10</t>
+  </si>
+  <si>
+    <t>A small window contain "Download Recipes from eCook Store" &amp; "Get Recipes from Local Directory" Buttons and a TextBox to insert URL pops up</t>
+  </si>
+  <si>
+    <t>Step 17</t>
+  </si>
+  <si>
+    <t>Repeat step 12</t>
+  </si>
+  <si>
+    <t>Same result as step 12</t>
+  </si>
+  <si>
+    <t>Step 18</t>
+  </si>
+  <si>
+    <t>In the filebrowser window, click on the "Cancel" or "Close" Button</t>
+  </si>
+  <si>
+    <t>It returns to the small window containing the two Buttons and TextBox instead of the Main Menu</t>
+  </si>
+  <si>
+    <t>Repeat steps 1-6. Now, move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, press the "Exit Slide" button on the Slide's Control Panel</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click the "Add Timer" button again</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Pause" Button on the Control Panel</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Play" Button on the Control Panel</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Add Timer" Button</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Previous" Button</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Next" Button</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click the "Previous Slide" Button or Left Arrow Key</t>
+  </si>
+  <si>
+    <t>Move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click the "Next Slide" Button or Right Arrow Key</t>
+  </si>
+  <si>
+    <t>The .txt file should display exactly what you have keyed into the notes panel.</t>
+  </si>
+  <si>
+    <t>Return to the Slideshow and move the mouse to the bottom of the window and wait for the Control Panel to slide up. Now, click on the "Next Slide" Button or Right Arrow Key</t>
+  </si>
+  <si>
+    <t>Navigate to the "Code" folder. Open up the eCook folder and under notes folder, search for the Recipe Title with its slide number ".txt file(Reciple Example #2_0). Double click on the .txt file.</t>
+  </si>
+  <si>
+    <t>Repeat steps 6-8. However, this time, search for "Reciple Example #2_1".txt file.</t>
+  </si>
+  <si>
+    <t>Modified Load External Recipes and Store Notes Instructions. Minor Changes to get the control panel as well.</t>
   </si>
 </sst>
 </file>
@@ -893,7 +953,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -998,6 +1058,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1273,7 +1336,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1281,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA176"/>
+  <dimension ref="A1:AA182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView topLeftCell="A163" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1362,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="11"/>
     </row>
@@ -1315,7 +1378,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1347,10 +1410,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="12"/>
     </row>
@@ -1359,10 +1422,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E6" s="12"/>
     </row>
@@ -1371,10 +1434,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E7" s="12"/>
     </row>
@@ -1383,10 +1446,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="12"/>
     </row>
@@ -1444,10 +1507,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="12"/>
     </row>
@@ -1456,10 +1519,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -1468,10 +1531,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -1480,10 +1543,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="12"/>
     </row>
@@ -1500,12 +1563,12 @@
       <c r="E18" s="12"/>
       <c r="F18" s="24"/>
     </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>13</v>
@@ -1518,7 +1581,7 @@
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="11"/>
     </row>
@@ -1564,10 +1627,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -1576,10 +1639,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E26" s="12"/>
     </row>
@@ -1588,10 +1651,10 @@
         <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E27" s="12"/>
     </row>
@@ -1600,10 +1663,10 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" s="12"/>
     </row>
@@ -1612,10 +1675,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E29" s="12"/>
     </row>
@@ -1625,7 +1688,7 @@
     </row>
     <row r="31" spans="1:6" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="11"/>
       <c r="E31" s="11"/>
@@ -1672,10 +1735,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="12"/>
     </row>
@@ -1684,10 +1747,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E36" s="12"/>
     </row>
@@ -1696,10 +1759,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E37" s="12"/>
     </row>
@@ -1708,10 +1771,10 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E38" s="12"/>
     </row>
@@ -1720,10 +1783,10 @@
         <v>8</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E39" s="12"/>
     </row>
@@ -1732,10 +1795,10 @@
         <v>9</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E40" s="12"/>
     </row>
@@ -1789,10 +1852,10 @@
         <v>4</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E46" s="12"/>
     </row>
@@ -1801,10 +1864,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E47" s="12"/>
     </row>
@@ -1813,34 +1876,34 @@
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E49" s="12"/>
     </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>24</v>
+        <v>171</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E50" s="12"/>
     </row>
@@ -1852,7 +1915,7 @@
         <v>15</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E51" s="12"/>
     </row>
@@ -1864,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E52" s="12"/>
     </row>
@@ -1874,7 +1937,7 @@
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E54" s="12"/>
     </row>
@@ -1920,10 +1983,10 @@
         <v>4</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E58" s="12"/>
     </row>
@@ -1932,10 +1995,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E59" s="12"/>
     </row>
@@ -1944,10 +2007,10 @@
         <v>6</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E60" s="12"/>
     </row>
@@ -1956,10 +2019,10 @@
         <v>7</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E61" s="12"/>
     </row>
@@ -1968,10 +2031,10 @@
         <v>8</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E62" s="12"/>
     </row>
@@ -1980,10 +2043,10 @@
         <v>9</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E63" s="12"/>
     </row>
@@ -1992,7 +2055,7 @@
     </row>
     <row r="65" spans="1:6" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E65" s="12"/>
     </row>
@@ -2036,10 +2099,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E69" s="12"/>
     </row>
@@ -2048,10 +2111,10 @@
         <v>5</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E70" s="12"/>
     </row>
@@ -2060,10 +2123,10 @@
         <v>6</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E71" s="12"/>
     </row>
@@ -2072,10 +2135,10 @@
         <v>7</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E72" s="12"/>
     </row>
@@ -2084,10 +2147,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E73" s="12"/>
     </row>
@@ -2096,10 +2159,10 @@
         <v>9</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="5"/>
@@ -2109,7 +2172,7 @@
     </row>
     <row r="76" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E76" s="12"/>
     </row>
@@ -2155,10 +2218,10 @@
         <v>4</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E80" s="12"/>
     </row>
@@ -2167,10 +2230,10 @@
         <v>5</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E81" s="12"/>
     </row>
@@ -2179,10 +2242,10 @@
         <v>6</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E82" s="12"/>
     </row>
@@ -2191,10 +2254,10 @@
         <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E83" s="12"/>
     </row>
@@ -2203,10 +2266,10 @@
         <v>8</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E84" s="12"/>
     </row>
@@ -2215,10 +2278,10 @@
         <v>9</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E85" s="12"/>
     </row>
@@ -2227,7 +2290,7 @@
     </row>
     <row r="87" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A87" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E87" s="12"/>
     </row>
@@ -2273,10 +2336,10 @@
         <v>4</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E91" s="12"/>
     </row>
@@ -2285,10 +2348,10 @@
         <v>5</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E92" s="12"/>
     </row>
@@ -2297,10 +2360,10 @@
         <v>6</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E93" s="12"/>
     </row>
@@ -2309,22 +2372,22 @@
         <v>7</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E94" s="12"/>
     </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E95" s="12"/>
     </row>
@@ -2333,10 +2396,10 @@
         <v>9</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E96" s="12"/>
       <c r="F96" s="5"/>
@@ -2346,7 +2409,7 @@
     </row>
     <row r="98" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E98" s="12"/>
     </row>
@@ -2438,10 +2501,10 @@
         <v>4</v>
       </c>
       <c r="B102" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D102" s="21"/>
       <c r="E102" s="12"/>
@@ -2473,10 +2536,10 @@
         <v>5</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E103" s="12"/>
     </row>
@@ -2485,22 +2548,22 @@
         <v>6</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E104" s="12"/>
     </row>
-    <row r="105" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>77</v>
+        <v>170</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D105" s="19"/>
       <c r="E105" s="12"/>
@@ -2532,10 +2595,10 @@
         <v>8</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D106" s="19"/>
       <c r="E106" s="12"/>
@@ -2567,10 +2630,10 @@
         <v>9</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D107" s="19"/>
       <c r="E107" s="12"/>
@@ -2602,10 +2665,10 @@
         <v>18</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D108" s="19"/>
       <c r="E108" s="12"/>
@@ -2634,13 +2697,13 @@
     </row>
     <row r="109" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D109" s="19"/>
       <c r="E109" s="12"/>
@@ -2669,13 +2732,13 @@
     </row>
     <row r="110" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D110" s="19"/>
       <c r="E110" s="12"/>
@@ -2702,15 +2765,15 @@
       <c r="Z110" s="19"/>
       <c r="AA110" s="19"/>
     </row>
-    <row r="111" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>69</v>
+        <v>167</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D111" s="19"/>
       <c r="E111" s="12"/>
@@ -2739,13 +2802,13 @@
     </row>
     <row r="112" spans="1:27" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D112" s="19"/>
       <c r="E112" s="12"/>
@@ -2772,15 +2835,15 @@
       <c r="Z112" s="19"/>
       <c r="AA112" s="19"/>
     </row>
-    <row r="113" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D113" s="19"/>
       <c r="E113" s="12"/>
@@ -2807,15 +2870,15 @@
       <c r="Z113" s="19"/>
       <c r="AA113" s="19"/>
     </row>
-    <row r="114" spans="1:27" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D114" s="19"/>
       <c r="E114" s="12"/>
@@ -2844,13 +2907,13 @@
     </row>
     <row r="115" spans="1:27" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D115" s="19"/>
       <c r="E115" s="12"/>
@@ -2882,7 +2945,7 @@
     </row>
     <row r="117" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E117" s="12"/>
     </row>
@@ -2928,10 +2991,10 @@
         <v>4</v>
       </c>
       <c r="B121" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E121" s="27"/>
     </row>
@@ -2940,10 +3003,10 @@
         <v>5</v>
       </c>
       <c r="B122" s="29" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E122" s="27"/>
     </row>
@@ -2952,10 +3015,10 @@
         <v>6</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E123" s="27"/>
     </row>
@@ -2964,10 +3027,10 @@
         <v>7</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E124" s="27"/>
     </row>
@@ -2976,10 +3039,10 @@
         <v>8</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E125" s="27"/>
     </row>
@@ -2988,10 +3051,10 @@
         <v>9</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E126" s="27"/>
     </row>
@@ -3000,70 +3063,70 @@
         <v>18</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E127" s="27"/>
     </row>
     <row r="128" spans="1:27" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B128" s="21" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E128" s="27"/>
     </row>
     <row r="129" spans="1:5" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E129" s="27"/>
     </row>
     <row r="130" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E130" s="27"/>
     </row>
     <row r="131" spans="1:5" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="18" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E131" s="27"/>
     </row>
     <row r="132" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B132" s="21" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E132" s="27"/>
     </row>
@@ -3072,7 +3135,7 @@
     </row>
     <row r="134" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A134" s="26" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E134" s="12"/>
     </row>
@@ -3118,10 +3181,10 @@
         <v>4</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C138" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E138" s="12"/>
     </row>
@@ -3130,10 +3193,10 @@
         <v>5</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E139" s="12"/>
     </row>
@@ -3142,10 +3205,10 @@
         <v>6</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E140" s="12"/>
     </row>
@@ -3154,10 +3217,10 @@
         <v>7</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E141" s="12"/>
     </row>
@@ -3166,52 +3229,52 @@
         <v>8</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E142" s="12"/>
     </row>
-    <row r="143" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="E143" s="12"/>
     </row>
-    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E144" s="12"/>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E145" s="12"/>
     </row>
     <row r="147" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E147" s="12"/>
     </row>
@@ -3257,10 +3320,10 @@
         <v>4</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C151" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E151" s="12"/>
     </row>
@@ -3269,10 +3332,10 @@
         <v>5</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3280,10 +3343,10 @@
         <v>6</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3291,10 +3354,10 @@
         <v>7</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3302,10 +3365,10 @@
         <v>8</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3313,10 +3376,10 @@
         <v>9</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3324,59 +3387,59 @@
         <v>18</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="163" spans="1:5" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A163" s="31" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E163" s="32"/>
     </row>
@@ -3393,62 +3456,64 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B165" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C165" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E165" s="32"/>
-    </row>
-    <row r="166" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B165" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C165" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="D165" s="34"/>
+      <c r="E165" s="33"/>
+    </row>
+    <row r="166" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B166" s="36" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C166" s="17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E166" s="32"/>
     </row>
-    <row r="167" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="33" t="s">
         <v>4</v>
       </c>
       <c r="B167" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C167" s="36" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="C167" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="E167" s="32"/>
     </row>
-    <row r="168" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B168" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="C168" s="35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B168" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C168" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E168" s="32"/>
+    </row>
+    <row r="169" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B169" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C169" s="35" t="s">
         <v>159</v>
-      </c>
-      <c r="C169" s="35" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="170" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3456,46 +3521,143 @@
         <v>7</v>
       </c>
       <c r="B170" s="35" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C170" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B171" s="35" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C171" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B172" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C172" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B173" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C173" s="35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A174" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B174" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C174" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A175" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B175" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C175" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B176" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C176" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B177" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C177" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A178" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B178" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C178" s="35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A179" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B179" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C179" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="C172" s="35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B175" s="3"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
+    </row>
+    <row r="180" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A180" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B180" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C180" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B181" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C181" s="35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A182" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B182" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C182" s="35" t="s">
+        <v>165</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3510,10 +3672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,16 +3688,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3546,10 +3708,10 @@
         <v>41685</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3560,10 +3722,10 @@
         <v>41772</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,10 +3736,10 @@
         <v>41773</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3588,10 +3750,10 @@
         <v>41781</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3602,10 +3764,24 @@
         <v>41784</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="B7" s="28">
+        <v>41786</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>